<commit_message>
Improved logic and added new file of containing raw data
</commit_message>
<xml_diff>
--- a/excel/statistics.xlsx
+++ b/excel/statistics.xlsx
@@ -128,9 +128,9 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>11</col>
       <colOff>0</colOff>
-      <row>60</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -153,9 +153,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>17</col>
       <colOff>0</colOff>
-      <row>60</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -178,9 +178,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>11</col>
       <colOff>0</colOff>
-      <row>84</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -203,9 +203,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>17</col>
       <colOff>0</colOff>
-      <row>84</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -228,9 +228,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>11</col>
       <colOff>0</colOff>
-      <row>108</row>
+      <row>37</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -253,9 +253,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>17</col>
       <colOff>0</colOff>
-      <row>108</row>
+      <row>37</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -280,7 +280,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>132</row>
+      <row>68</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -305,7 +305,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>154</row>
+      <row>93</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -330,7 +330,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>176</row>
+      <row>118</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -355,7 +355,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>198</row>
+      <row>143</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -380,7 +380,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>220</row>
+      <row>168</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -693,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I219"/>
+  <dimension ref="A1:L166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -747,6 +747,11 @@
           <t>iou_std</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Mean and Std Dev</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1413,6 +1418,11 @@
       <c r="I19" t="n">
         <v/>
       </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Box Plot</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2079,6 +2089,11 @@
       <c r="I37" t="n">
         <v/>
       </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Rolling Mean</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2746,72 +2761,48 @@
         <v>0.07711207149862898</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Mean and Std Dev</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Box Plot</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Rolling Mean</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
+    <row r="66">
+      <c r="A66" t="inlineStr">
         <is>
           <t>Task Comparison (Accuracy)</t>
         </is>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
+    <row r="91">
+      <c r="A91" t="inlineStr">
         <is>
           <t>Task Comparison (IoU)</t>
         </is>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
+    <row r="116">
+      <c r="A116" t="inlineStr">
         <is>
           <t>Correlation Heatmap</t>
         </is>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
+    <row r="141">
+      <c r="A141" t="inlineStr">
         <is>
           <t>Time vs Accuracy</t>
         </is>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
+    <row r="166">
+      <c r="A166" t="inlineStr">
         <is>
           <t>Time vs IoU</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A131:H131"/>
-    <mergeCell ref="A153:H153"/>
-    <mergeCell ref="A83:H83"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A107:H107"/>
-    <mergeCell ref="A175:H175"/>
-    <mergeCell ref="A219:H219"/>
-    <mergeCell ref="A197:H197"/>
+  <mergeCells count="5">
+    <mergeCell ref="A91:H91"/>
+    <mergeCell ref="A166:H166"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="A141:H141"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Added plots for the raw data
</commit_message>
<xml_diff>
--- a/excel/statistics.xlsx
+++ b/excel/statistics.xlsx
@@ -178,9 +178,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>11</col>
+      <col>23</col>
       <colOff>0</colOff>
-      <row>19</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -203,7 +203,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>17</col>
+      <col>11</col>
       <colOff>0</colOff>
       <row>19</row>
       <rowOff>0</rowOff>
@@ -228,9 +228,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>11</col>
+      <col>17</col>
       <colOff>0</colOff>
-      <row>37</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -253,9 +253,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>17</col>
+      <col>23</col>
       <colOff>0</colOff>
-      <row>37</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -278,9 +278,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>11</col>
       <colOff>0</colOff>
-      <row>68</row>
+      <row>37</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -303,9 +303,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>17</col>
       <colOff>0</colOff>
-      <row>93</row>
+      <row>37</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -328,9 +328,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>23</col>
       <colOff>0</colOff>
-      <row>118</row>
+      <row>37</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -353,9 +353,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>21</col>
       <colOff>0</colOff>
-      <row>143</row>
+      <row>59</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -378,9 +378,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>0</col>
+      <col>21</col>
       <colOff>0</colOff>
-      <row>168</row>
+      <row>83</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="3810000" cy="2857500"/>
@@ -391,6 +391,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>21</col>
+      <colOff>0</colOff>
+      <row>107</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="2857500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -693,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L166"/>
+  <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,13 +795,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.3981615458937198</v>
+        <v>0.395702515137401</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1398982485983164</v>
+        <v>0.1406529428055432</v>
       </c>
       <c r="F2" t="n">
-        <v>147639590506.3429</v>
+        <v>141863172318.9341</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -807,13 +832,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5180021276595744</v>
+        <v>0.5238194805194805</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2183667591853526</v>
+        <v>0.2066462869373407</v>
       </c>
       <c r="F3" t="n">
-        <v>1289244187171.085</v>
+        <v>1127692693324.948</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -844,13 +869,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.5233911111111111</v>
+        <v>0.53038</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2116318102294882</v>
+        <v>0.2015162242814426</v>
       </c>
       <c r="F4" t="n">
-        <v>1393852674580.733</v>
+        <v>1221178546075.347</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -881,13 +906,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.5261217391304348</v>
+        <v>0.5357776315789473</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2173700111310906</v>
+        <v>0.2069669330102012</v>
       </c>
       <c r="F5" t="n">
-        <v>1561774191198.609</v>
+        <v>1359519905000.921</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -918,13 +943,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.54284</v>
+        <v>0.5464760000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2077481598211905</v>
+        <v>0.1983665988122101</v>
       </c>
       <c r="F6" t="n">
-        <v>1647422155839.378</v>
+        <v>1443319379853.133</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -955,13 +980,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5351488888888889</v>
+        <v>0.5447386666666667</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2169349154828599</v>
+        <v>0.2044098862403499</v>
       </c>
       <c r="F7" t="n">
-        <v>1821858329640.089</v>
+        <v>1583163532589.2</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -992,13 +1017,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.5344454545454546</v>
+        <v>0.5440891891891891</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2183468964472834</v>
+        <v>0.207256798270818</v>
       </c>
       <c r="F8" t="n">
-        <v>1860617139874.795</v>
+        <v>1638335764204.432</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1029,13 +1054,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.5427636363636363</v>
+        <v>0.5551797297297297</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2178571786167292</v>
+        <v>0.2065717932048593</v>
       </c>
       <c r="F9" t="n">
-        <v>1984682784236.409</v>
+        <v>1747671191657.513</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1066,13 +1091,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.5525534883720929</v>
+        <v>0.5599808219178082</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2118766345337565</v>
+        <v>0.2005621867107654</v>
       </c>
       <c r="F10" t="n">
-        <v>2121393075604.977</v>
+        <v>1861041395419.712</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1103,13 +1128,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.552153488372093</v>
+        <v>0.5622739726027397</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2154584407488425</v>
+        <v>0.202457238302175</v>
       </c>
       <c r="F11" t="n">
-        <v>2246099448200.326</v>
+        <v>1970544057279.548</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1140,13 +1165,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.5592069767441861</v>
+        <v>0.5675287671232877</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2133928184128185</v>
+        <v>0.2035992226569504</v>
       </c>
       <c r="F12" t="n">
-        <v>2370956429083.582</v>
+        <v>2080133082254.069</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1177,13 +1202,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.5291471518987342</v>
+        <v>0.5230260133091349</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1584370933540013</v>
+        <v>0.1613087964420446</v>
       </c>
       <c r="F13" t="n">
-        <v>332815247086.0465</v>
+        <v>281706336983.4059</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1214,13 +1239,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.5634651162790697</v>
+        <v>0.5724684931506849</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2170548239760998</v>
+        <v>0.2043775359181523</v>
       </c>
       <c r="F14" t="n">
-        <v>2495827491128.768</v>
+        <v>2189770455562.274</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1251,13 +1276,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5667558139534884</v>
+        <v>0.5758109589041096</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2133545956320086</v>
+        <v>0.2011229471697211</v>
       </c>
       <c r="F15" t="n">
-        <v>2620836616374.604</v>
+        <v>2299711902643.822</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1288,13 +1313,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.5701357142857143</v>
+        <v>0.5756323943661972</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2168439517835052</v>
+        <v>0.203360791820595</v>
       </c>
       <c r="F16" t="n">
-        <v>2784782409399.167</v>
+        <v>2403946219823.422</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1325,13 +1350,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.5702904761904762</v>
+        <v>0.5762295774647888</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2171608314967344</v>
+        <v>0.205024717948395</v>
       </c>
       <c r="F17" t="n">
-        <v>2911494643800.5</v>
+        <v>2513565414321.338</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1362,13 +1387,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.5759268292682926</v>
+        <v>0.5816225352112676</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2173295286246099</v>
+        <v>0.2063881566350045</v>
       </c>
       <c r="F18" t="n">
-        <v>3010863430493.049</v>
+        <v>2623244229421.845</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1399,13 +1424,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.5763487804878048</v>
+        <v>0.5845464788732394</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2161828660208195</v>
+        <v>0.2002092661127965</v>
       </c>
       <c r="F19" t="n">
-        <v>3136387026800.708</v>
+        <v>2732667152708.93</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1441,13 +1466,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.5732926829268292</v>
+        <v>0.5830352112676056</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2169292769432516</v>
+        <v>0.2026586151977836</v>
       </c>
       <c r="F20" t="n">
-        <v>3261832098284.902</v>
+        <v>2842042367972.169</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1478,13 +1503,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.5818634146341464</v>
+        <v>0.5911521126760564</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2140589588829414</v>
+        <v>0.1985937438657515</v>
       </c>
       <c r="F21" t="n">
-        <v>3387648317333.024</v>
+        <v>2951680040124.282</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1515,13 +1540,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.5839749999999999</v>
+        <v>0.59363</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2182762807626833</v>
+        <v>0.2014748650846292</v>
       </c>
       <c r="F22" t="n">
-        <v>3518339515546.525</v>
+        <v>3057450097014.872</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1552,13 +1577,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.5918615384615384</v>
+        <v>0.5990420289855073</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2173478858461277</v>
+        <v>0.198616145014771</v>
       </c>
       <c r="F23" t="n">
-        <v>3676820916931.18</v>
+        <v>3178416529847.667</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1589,13 +1614,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.4662648</v>
+        <v>0.4549147959183674</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1831722612716097</v>
+        <v>0.1792837236751567</v>
       </c>
       <c r="F24" t="n">
-        <v>436526631264.096</v>
+        <v>384536352740.0408</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1626,13 +1651,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.5883282051282052</v>
+        <v>0.5981623188405798</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2197295885361656</v>
+        <v>0.2008367255358334</v>
       </c>
       <c r="F25" t="n">
-        <v>3803714971484.539</v>
+        <v>3288087994260.855</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1663,13 +1688,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.5916461538461538</v>
+        <v>0.6001159420289855</v>
       </c>
       <c r="E26" t="n">
-        <v>0.2162040153068805</v>
+        <v>0.1983371450950809</v>
       </c>
       <c r="F26" t="n">
-        <v>3930521561838.205</v>
+        <v>3397721378163.261</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1700,13 +1725,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.5969564102564103</v>
+        <v>0.6040768115942029</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2160283300072516</v>
+        <v>0.1980560475819969</v>
       </c>
       <c r="F27" t="n">
-        <v>4057378401047.615</v>
+        <v>3507526190011.377</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1737,13 +1762,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.5985615384615385</v>
+        <v>0.6056420289855072</v>
       </c>
       <c r="E28" t="n">
-        <v>0.2178715829099245</v>
+        <v>0.198599638947155</v>
       </c>
       <c r="F28" t="n">
-        <v>4184530556878.897</v>
+        <v>3617470476536.102</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1774,13 +1799,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.5969589743589744</v>
+        <v>0.6063710144927535</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2178149549236555</v>
+        <v>0.1973265844030929</v>
       </c>
       <c r="F29" t="n">
-        <v>4311396066258.641</v>
+        <v>3727147406226.522</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1811,13 +1836,13 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.5935263157894737</v>
+        <v>0.6035955882352941</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2154080510982624</v>
+        <v>0.195601171618308</v>
       </c>
       <c r="F30" t="n">
-        <v>4187464999833.658</v>
+        <v>3687795850945.529</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1848,13 +1873,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.5922078947368421</v>
+        <v>0.6045867647058824</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2147982490008391</v>
+        <v>0.194410256243492</v>
       </c>
       <c r="F31" t="n">
-        <v>4307013744359.526</v>
+        <v>3793148879566.191</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1885,13 +1910,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.5964947368421052</v>
+        <v>0.6077867647058824</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2148894925900393</v>
+        <v>0.1949663437502657</v>
       </c>
       <c r="F32" t="n">
-        <v>4426718202651.263</v>
+        <v>3898587515188.338</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1922,13 +1947,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.5915473684210526</v>
+        <v>0.606185294117647</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2140357569733569</v>
+        <v>0.1942045054311639</v>
       </c>
       <c r="F33" t="n">
-        <v>4546289930433.132</v>
+        <v>4003947365611.162</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1959,13 +1984,13 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.600372972972973</v>
+        <v>0.6106805970149254</v>
       </c>
       <c r="E34" t="n">
-        <v>0.2136989349641332</v>
+        <v>0.1930700808850805</v>
       </c>
       <c r="F34" t="n">
-        <v>3520643544640.514</v>
+        <v>3468530106897.403</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1996,13 +2021,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.4799015748031496</v>
+        <v>0.4741370558375634</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1977286592679802</v>
+        <v>0.1897267761525686</v>
       </c>
       <c r="F35" t="n">
-        <v>608729763949.3544</v>
+        <v>531209346349.8883</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2033,13 +2058,13 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.6019891891891892</v>
+        <v>0.6130089552238807</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2151226649867256</v>
+        <v>0.1946008391175525</v>
       </c>
       <c r="F36" t="n">
-        <v>3610803491023.027</v>
+        <v>3557208080952.522</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2070,13 +2095,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.6057162162162162</v>
+        <v>0.6172611940298507</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2140528588839598</v>
+        <v>0.192883019937917</v>
       </c>
       <c r="F37" t="n">
-        <v>3701107398423.297</v>
+        <v>3646145856666.925</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2112,13 +2137,13 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.6016297297297297</v>
+        <v>0.612341791044776</v>
       </c>
       <c r="E38" t="n">
-        <v>0.2163839063445453</v>
+        <v>0.194068369044031</v>
       </c>
       <c r="F38" t="n">
-        <v>3791568613881.892</v>
+        <v>3735178105362.179</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2149,13 +2174,13 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.6018081081081081</v>
+        <v>0.6149402985074627</v>
       </c>
       <c r="E39" t="n">
-        <v>0.2157799012089999</v>
+        <v>0.1930936780501626</v>
       </c>
       <c r="F39" t="n">
-        <v>3881803872287.297</v>
+        <v>3823884921871.985</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2186,13 +2211,13 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.6043756756756756</v>
+        <v>0.614120895522388</v>
       </c>
       <c r="E40" t="n">
-        <v>0.2164397470755178</v>
+        <v>0.1920223223587153</v>
       </c>
       <c r="F40" t="n">
-        <v>3971869125140.459</v>
+        <v>3912680876316.925</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2223,13 +2248,13 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.6034918918918919</v>
+        <v>0.6151402985074627</v>
       </c>
       <c r="E41" t="n">
-        <v>0.2124980789173012</v>
+        <v>0.1897548714268294</v>
       </c>
       <c r="F41" t="n">
-        <v>4062115952176.811</v>
+        <v>4001392447919.433</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2260,13 +2285,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.6068324324324325</v>
+        <v>0.6173223880597014</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2113403574727191</v>
+        <v>0.1898599753733162</v>
       </c>
       <c r="F42" t="n">
-        <v>4152215785975.648</v>
+        <v>4090261830884.493</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2297,13 +2322,13 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.6050891891891892</v>
+        <v>0.6184388059701492</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2155610222751885</v>
+        <v>0.1922325280354923</v>
       </c>
       <c r="F43" t="n">
-        <v>4242499065379.108</v>
+        <v>4179177438112.612</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2334,13 +2359,13 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.6119864864864865</v>
+        <v>0.6196776119402985</v>
       </c>
       <c r="E44" t="n">
-        <v>0.2124219793531553</v>
+        <v>0.1901408910007902</v>
       </c>
       <c r="F44" t="n">
-        <v>4332799256874.433</v>
+        <v>4268140530208.089</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2371,13 +2396,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.6077648648648649</v>
+        <v>0.6212089552238806</v>
       </c>
       <c r="E45" t="n">
-        <v>0.2160889685808657</v>
+        <v>0.191924786981731</v>
       </c>
       <c r="F45" t="n">
-        <v>4423258174312.595</v>
+        <v>4357217364261.552</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2408,13 +2433,13 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.6415520084566596</v>
+        <v>0.6340570852921423</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1849287151987505</v>
+        <v>0.1878002288590449</v>
       </c>
       <c r="F46" t="n">
-        <v>629461503055.424</v>
+        <v>578762791544.2616</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2445,13 +2470,13 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.6084189189189189</v>
+        <v>0.6225373134328358</v>
       </c>
       <c r="E47" t="n">
-        <v>0.216372883952472</v>
+        <v>0.1921749091526376</v>
       </c>
       <c r="F47" t="n">
-        <v>4513635572675.162</v>
+        <v>4445962670216.09</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2482,13 +2507,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.4851</v>
+        <v>0.486093670886076</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2077892391743775</v>
+        <v>0.1973441685403059</v>
       </c>
       <c r="F48" t="n">
-        <v>765787114862.2858</v>
+        <v>674386712737.405</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2519,13 +2544,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.5004775510204081</v>
+        <v>0.5011050632911392</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2137969161623811</v>
+        <v>0.2034270983251955</v>
       </c>
       <c r="F49" t="n">
-        <v>893416854901.6123</v>
+        <v>786679154081.2911</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2556,13 +2581,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.5042163265306123</v>
+        <v>0.5088746835443038</v>
       </c>
       <c r="E50" t="n">
-        <v>0.2214071074466471</v>
+        <v>0.206412460161286</v>
       </c>
       <c r="F50" t="n">
-        <v>1066689965566.061</v>
+        <v>927245494005.8228</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2593,13 +2618,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.5234446808510639</v>
+        <v>0.5248103896103896</v>
       </c>
       <c r="E51" t="n">
-        <v>0.2180539071846292</v>
+        <v>0.2058806377391979</v>
       </c>
       <c r="F51" t="n">
-        <v>1119802442228.362</v>
+        <v>990240688644.7533</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2616,12 +2641,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>img-segmentation</t>
+          <t>img-classification</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>coco</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2630,35 +2655,35 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v/>
+        <v>0.77711</v>
       </c>
       <c r="E52" t="n">
-        <v/>
+        <v>0.309537671195105</v>
       </c>
       <c r="F52" t="n">
-        <v>463115153103.0793</v>
+        <v>154872496903.5</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>iou</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>0.1371973445039648</v>
+        <v/>
       </c>
       <c r="I52" t="n">
-        <v>0.09761506414197786</v>
+        <v/>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>img-segmentation</t>
+          <t>img-classification</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>coco</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2667,35 +2692,35 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v/>
+        <v>0.911675</v>
       </c>
       <c r="E53" t="n">
-        <v/>
+        <v>0.1039321585046157</v>
       </c>
       <c r="F53" t="n">
-        <v>1023305817031.333</v>
+        <v>352057443182.5</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>iou</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>0.1935871668344687</v>
+        <v/>
       </c>
       <c r="I53" t="n">
-        <v>0.1124989292573845</v>
+        <v/>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>img-segmentation</t>
+          <t>img-classification</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>coco</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2704,106 +2729,1966 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v/>
+        <v>0.9298125</v>
       </c>
       <c r="E54" t="n">
-        <v/>
+        <v>0.1180992129827411</v>
       </c>
       <c r="F54" t="n">
-        <v>1517097922323.556</v>
+        <v>519572164456.375</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>iou</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>0.05424617065323724</v>
+        <v/>
       </c>
       <c r="I54" t="n">
-        <v>0.02697025015868808</v>
+        <v/>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>img-segmentation</t>
+          <t>img-classification</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>coco</t>
+          <t>mnist</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.9244875</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.1338583733172597</v>
+      </c>
+      <c r="F55" t="n">
+        <v>702967018547.875</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v/>
+      </c>
+      <c r="I55" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>img-classification</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>mnist</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D55" t="n">
-        <v/>
-      </c>
-      <c r="E55" t="n">
-        <v/>
-      </c>
-      <c r="F55" t="n">
-        <v/>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>iou</t>
-        </is>
-      </c>
-      <c r="H55" t="n">
-        <v>0.229677390307188</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0.07711207149862898</v>
+      <c r="D56" t="n">
+        <v>0.9813571428571429</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.01254284087210141</v>
+      </c>
+      <c r="F56" t="n">
+        <v>876284113852.7142</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v/>
+      </c>
+      <c r="I56" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v/>
+      </c>
+      <c r="E57" t="n">
+        <v/>
+      </c>
+      <c r="F57" t="n">
+        <v>450030999349.2929</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>0.1704422620811848</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.03696675884396014</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v/>
+      </c>
+      <c r="E58" t="n">
+        <v/>
+      </c>
+      <c r="F58" t="n">
+        <v>2968583564771.3</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>0.1861270412802696</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.07171408386126632</v>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>Correlation Heatmap</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v/>
+      </c>
+      <c r="E59" t="n">
+        <v/>
+      </c>
+      <c r="F59" t="n">
+        <v>3265457753721.6</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>0.1898500710725784</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.07106446594183173</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v/>
+      </c>
+      <c r="E60" t="n">
+        <v/>
+      </c>
+      <c r="F60" t="n">
+        <v>3533963251235</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>0.1759520918130875</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.06801957307046885</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v/>
+      </c>
+      <c r="E61" t="n">
+        <v/>
+      </c>
+      <c r="F61" t="n">
+        <v>3828652907036</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>0.1765054706484079</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.07160925999704425</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v/>
+      </c>
+      <c r="E62" t="n">
+        <v/>
+      </c>
+      <c r="F62" t="n">
+        <v>4122833071393.75</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>0.1916059423238039</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.07428610056954099</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v/>
+      </c>
+      <c r="E63" t="n">
+        <v/>
+      </c>
+      <c r="F63" t="n">
+        <v>4417558874926.25</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>0.1745931748300791</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.06774357413870717</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v/>
+      </c>
+      <c r="E64" t="n">
+        <v/>
+      </c>
+      <c r="F64" t="n">
+        <v>4712407760743.875</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>0.1728480234742165</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.06324201895881346</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v/>
+      </c>
+      <c r="E65" t="n">
+        <v/>
+      </c>
+      <c r="F65" t="n">
+        <v>5006784091093.125</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>0.1787202432751656</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.07144190205365576</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Task Comparison (Accuracy)</t>
-        </is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v/>
+      </c>
+      <c r="E66" t="n">
+        <v/>
+      </c>
+      <c r="F66" t="n">
+        <v>5300337760181.75</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>0.1772708464413881</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.07427959868907347</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v/>
+      </c>
+      <c r="E67" t="n">
+        <v/>
+      </c>
+      <c r="F67" t="n">
+        <v>5595064558115.375</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>0.1805790401995182</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.07130951380382484</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v/>
+      </c>
+      <c r="E68" t="n">
+        <v/>
+      </c>
+      <c r="F68" t="n">
+        <v>902237670536.1034</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>0.1881771329148062</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.05503870824255786</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v/>
+      </c>
+      <c r="E69" t="n">
+        <v/>
+      </c>
+      <c r="F69" t="n">
+        <v>5889667881883.875</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>0.1801694761961699</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.07667292930994277</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v/>
+      </c>
+      <c r="E70" t="n">
+        <v/>
+      </c>
+      <c r="F70" t="n">
+        <v>6182734295294</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>0.1760056354105473</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.08067729251053302</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v/>
+      </c>
+      <c r="E71" t="n">
+        <v/>
+      </c>
+      <c r="F71" t="n">
+        <v>6477559698751.125</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>0.1758031323552132</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.07191769812928017</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v/>
+      </c>
+      <c r="E72" t="n">
+        <v/>
+      </c>
+      <c r="F72" t="n">
+        <v>6771318662562.5</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>0.1918547283858061</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.07196120565196328</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v/>
+      </c>
+      <c r="E73" t="n">
+        <v/>
+      </c>
+      <c r="F73" t="n">
+        <v>7066344752603.5</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>0.1882986146956682</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.07713970785263573</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v/>
+      </c>
+      <c r="E74" t="n">
+        <v/>
+      </c>
+      <c r="F74" t="n">
+        <v>7360526291942.75</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>0.1826615128666162</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.07650291744537038</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v/>
+      </c>
+      <c r="E75" t="n">
+        <v/>
+      </c>
+      <c r="F75" t="n">
+        <v>7655673648697.5</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>0.2026659771800041</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.08096076207633401</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v/>
+      </c>
+      <c r="E76" t="n">
+        <v/>
+      </c>
+      <c r="F76" t="n">
+        <v>7951171910612.25</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>0.1917365342378616</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.06875768964030336</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v/>
+      </c>
+      <c r="E77" t="n">
+        <v/>
+      </c>
+      <c r="F77" t="n">
+        <v>8246255078848.5</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>0.1811824291944504</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.07746239955041412</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v/>
+      </c>
+      <c r="E78" t="n">
+        <v/>
+      </c>
+      <c r="F78" t="n">
+        <v>8540586175314.375</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>0.1894466802477837</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.07758982067393008</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v/>
+      </c>
+      <c r="E79" t="n">
+        <v/>
+      </c>
+      <c r="F79" t="n">
+        <v>1314243230883.869</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H79" t="n">
+        <v>0.2001151572025958</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.06449737283652171</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v/>
+      </c>
+      <c r="E80" t="n">
+        <v/>
+      </c>
+      <c r="F80" t="n">
+        <v>8835506630048.125</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H80" t="n">
+        <v>0.1947078965604305</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.07726817402985407</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v/>
+      </c>
+      <c r="E81" t="n">
+        <v/>
+      </c>
+      <c r="F81" t="n">
+        <v>9130049005602.75</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H81" t="n">
+        <v>0.1860596518963575</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.0751374060370233</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v/>
+      </c>
+      <c r="E82" t="n">
+        <v/>
+      </c>
+      <c r="F82" t="n">
+        <v>9425610649249.375</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H82" t="n">
+        <v>0.1834042314440012</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.07412066476728382</v>
+      </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>Time vs Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v/>
+      </c>
+      <c r="E83" t="n">
+        <v/>
+      </c>
+      <c r="F83" t="n">
+        <v>9720738562145.25</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>0.1830331943929195</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.07274024305692223</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v/>
+      </c>
+      <c r="E84" t="n">
+        <v/>
+      </c>
+      <c r="F84" t="n">
+        <v>10014985168236.88</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H84" t="n">
+        <v>0.1986057981848717</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.07809313348605283</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v/>
+      </c>
+      <c r="E85" t="n">
+        <v/>
+      </c>
+      <c r="F85" t="n">
+        <v>10309757161148.62</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>0.1833901442587376</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.07000445209643377</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v/>
+      </c>
+      <c r="E86" t="n">
+        <v/>
+      </c>
+      <c r="F86" t="n">
+        <v>10604356547791.62</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H86" t="n">
+        <v>0.2031211648136377</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.07934894647071287</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v/>
+      </c>
+      <c r="E87" t="n">
+        <v/>
+      </c>
+      <c r="F87" t="n">
+        <v>10898430868917.88</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H87" t="n">
+        <v>0.1832808572798967</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0.07320571540825345</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v/>
+      </c>
+      <c r="E88" t="n">
+        <v/>
+      </c>
+      <c r="F88" t="n">
+        <v>11192850655253.25</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H88" t="n">
+        <v>0.2015318423509598</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0.07367139459852201</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v/>
+      </c>
+      <c r="E89" t="n">
+        <v/>
+      </c>
+      <c r="F89" t="n">
+        <v>11487881847928.25</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H89" t="n">
+        <v>0.1930310986936092</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.06849543101099262</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v/>
+      </c>
+      <c r="E90" t="n">
+        <v/>
+      </c>
+      <c r="F90" t="n">
+        <v>1745317392389.729</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H90" t="n">
+        <v>0.2107047968051013</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.07820927095547602</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Task Comparison (IoU)</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>Correlation Heatmap</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Time vs Accuracy</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v/>
+      </c>
+      <c r="E91" t="n">
+        <v/>
+      </c>
+      <c r="F91" t="n">
+        <v>11782250415032.88</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H91" t="n">
+        <v>0.1859051492065191</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.07266640491454728</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v/>
+      </c>
+      <c r="E92" t="n">
+        <v/>
+      </c>
+      <c r="F92" t="n">
+        <v>12076338097233.5</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H92" t="n">
+        <v>0.1851323656737804</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0.07388562128693886</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v/>
+      </c>
+      <c r="E93" t="n">
+        <v/>
+      </c>
+      <c r="F93" t="n">
+        <v>12371093313572.25</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H93" t="n">
+        <v>0.2013100646436214</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.07694136391408077</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v/>
+      </c>
+      <c r="E94" t="n">
+        <v/>
+      </c>
+      <c r="F94" t="n">
+        <v>12664229246068.62</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H94" t="n">
+        <v>0.1888273973017931</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0.07223331889360922</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v/>
+      </c>
+      <c r="E95" t="n">
+        <v/>
+      </c>
+      <c r="F95" t="n">
+        <v>12959012243525.38</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H95" t="n">
+        <v>0.1938723269850016</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.07142377466069931</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v/>
+      </c>
+      <c r="E96" t="n">
+        <v/>
+      </c>
+      <c r="F96" t="n">
+        <v>13254366729402.88</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H96" t="n">
+        <v>0.1829858161509037</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.07307022546493488</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v/>
+      </c>
+      <c r="E97" t="n">
+        <v/>
+      </c>
+      <c r="F97" t="n">
+        <v>13549649047011.5</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H97" t="n">
+        <v>0.1999342571943998</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.07334878742128237</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v/>
+      </c>
+      <c r="E98" t="n">
+        <v/>
+      </c>
+      <c r="F98" t="n">
+        <v>13884469149822.86</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H98" t="n">
+        <v>0.187964283994266</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0.07700873921217133</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v/>
+      </c>
+      <c r="E99" t="n">
+        <v/>
+      </c>
+      <c r="F99" t="n">
+        <v>14180589981977.43</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H99" t="n">
+        <v>0.1948428196566445</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0.07415046473381895</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v/>
+      </c>
+      <c r="E100" t="n">
+        <v/>
+      </c>
+      <c r="F100" t="n">
+        <v>14475943991165</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>0.1905131680624826</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.07981155148283595</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v/>
+      </c>
+      <c r="E101" t="n">
+        <v/>
+      </c>
+      <c r="F101" t="n">
+        <v>2189602599767.786</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>0.2172274296837194</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.08401351498492113</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v/>
+      </c>
+      <c r="E102" t="n">
+        <v/>
+      </c>
+      <c r="F102" t="n">
+        <v>14771778885317.57</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H102" t="n">
+        <v>0.202729657292366</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.07783139757129603</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v/>
+      </c>
+      <c r="E103" t="n">
+        <v/>
+      </c>
+      <c r="F103" t="n">
+        <v>1828109571803.636</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H103" t="n">
+        <v>0.1827357126907869</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0.06490658907691857</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v/>
+      </c>
+      <c r="E104" t="n">
+        <v/>
+      </c>
+      <c r="F104" t="n">
+        <v>2132214648603.455</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>0.1869625300168991</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0.07385404112544985</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v/>
+      </c>
+      <c r="E105" t="n">
+        <v/>
+      </c>
+      <c r="F105" t="n">
+        <v>2436959358794.455</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>0.1852527436884967</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0.08030021051221893</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>img-segmentation</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v/>
+      </c>
+      <c r="E106" t="n">
+        <v/>
+      </c>
+      <c r="F106" t="n">
+        <v>2671802437954</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>iou</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>0.1611605532467365</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0.06760391955079546</v>
+      </c>
+      <c r="V106" t="inlineStr">
         <is>
           <t>Time vs IoU</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A91:H91"/>
-    <mergeCell ref="A166:H166"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="A116:H116"/>
-    <mergeCell ref="A141:H141"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Project structure aligned with AB projects.
</commit_message>
<xml_diff>
--- a/excel/statistics.xlsx
+++ b/excel/statistics.xlsx
@@ -795,13 +795,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.395702515137401</v>
+        <v>0.3956729515828677</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1406529428055432</v>
+        <v>0.1406268584264503</v>
       </c>
       <c r="F2" t="n">
-        <v>141863172318.9341</v>
+        <v>141645697853.1395</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5238194805194805</v>
+        <v>0.5257717948717948</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2066462869373407</v>
+        <v>0.2060228312259274</v>
       </c>
       <c r="F3" t="n">
-        <v>1127692693324.948</v>
+        <v>1113584289929.833</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -869,13 +869,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.53038</v>
+        <v>0.5323763157894736</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2015162242814426</v>
+        <v>0.200923416168729</v>
       </c>
       <c r="F4" t="n">
-        <v>1221178546075.347</v>
+        <v>1205503821556.079</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -906,13 +906,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.5357776315789473</v>
+        <v>0.5377090909090909</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2069669330102012</v>
+        <v>0.2062981823668035</v>
       </c>
       <c r="F5" t="n">
-        <v>1359519905000.921</v>
+        <v>1342287262533.286</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -943,13 +943,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.5464760000000001</v>
+        <v>0.5482907894736841</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1983665988122101</v>
+        <v>0.1976738554134944</v>
       </c>
       <c r="F6" t="n">
-        <v>1443319379853.133</v>
+        <v>1424792523738.25</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -980,13 +980,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5447386666666667</v>
+        <v>0.5465671052631579</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2044098862403499</v>
+        <v>0.2036673067451969</v>
       </c>
       <c r="F7" t="n">
-        <v>1583163532589.2</v>
+        <v>1562831919165.171</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1017,13 +1017,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.5440891891891891</v>
+        <v>0.5459506666666667</v>
       </c>
       <c r="E8" t="n">
-        <v>0.207256798270818</v>
+        <v>0.2064819234109743</v>
       </c>
       <c r="F8" t="n">
-        <v>1638335764204.432</v>
+        <v>1617033360696.32</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1054,13 +1054,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.5551797297297297</v>
+        <v>0.5568960000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2065717932048593</v>
+        <v>0.2057089622402143</v>
       </c>
       <c r="F9" t="n">
-        <v>1747671191657.513</v>
+        <v>1724946791383.813</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1091,13 +1091,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.5599808219178082</v>
+        <v>0.5616594594594595</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2005621867107654</v>
+        <v>0.1997064838802521</v>
       </c>
       <c r="F10" t="n">
-        <v>1861041395419.712</v>
+        <v>1836514193219.297</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.5622739726027397</v>
+        <v>0.5639378378378378</v>
       </c>
       <c r="E11" t="n">
-        <v>0.202457238302175</v>
+        <v>0.2015745673936039</v>
       </c>
       <c r="F11" t="n">
-        <v>1970544057279.548</v>
+        <v>1944573126475.581</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1165,13 +1165,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.5675287671232877</v>
+        <v>0.5690986486486487</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2035992226569504</v>
+        <v>0.2026503740626646</v>
       </c>
       <c r="F12" t="n">
-        <v>2080133082254.069</v>
+        <v>2052717496138.013</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1202,13 +1202,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.5230260133091349</v>
+        <v>0.5230296856106409</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1613087964420446</v>
+        <v>0.1612600654810651</v>
       </c>
       <c r="F13" t="n">
-        <v>281706336983.4059</v>
+        <v>280347162297.0295</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.5724684931506849</v>
+        <v>0.5739716216216216</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2043775359181523</v>
+        <v>0.2033843116484937</v>
       </c>
       <c r="F14" t="n">
-        <v>2189770455562.274</v>
+        <v>2160909321594.906</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1276,13 +1276,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5758109589041096</v>
+        <v>0.5772716216216216</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2011229471697211</v>
+        <v>0.2001354688603808</v>
       </c>
       <c r="F15" t="n">
-        <v>2299711902643.822</v>
+        <v>2269401210093.243</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1313,13 +1313,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.5756323943661972</v>
+        <v>0.5771333333333334</v>
       </c>
       <c r="E16" t="n">
-        <v>0.203360791820595</v>
+        <v>0.2023248406072783</v>
       </c>
       <c r="F16" t="n">
-        <v>2403946219823.422</v>
+        <v>2371383336712.25</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1350,13 +1350,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.5762295774647888</v>
+        <v>0.5777222222222222</v>
       </c>
       <c r="E17" t="n">
-        <v>0.205024717948395</v>
+        <v>0.2039693750985445</v>
       </c>
       <c r="F17" t="n">
-        <v>2513565414321.338</v>
+        <v>2479517378536.597</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1387,13 +1387,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.5816225352112676</v>
+        <v>0.5830319444444444</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2063881566350045</v>
+        <v>0.2052782253680366</v>
       </c>
       <c r="F18" t="n">
-        <v>2623244229421.845</v>
+        <v>2587709937089.431</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1424,13 +1424,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.5845464788732394</v>
+        <v>0.5859319444444444</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2002092661127965</v>
+        <v>0.1991416466840957</v>
       </c>
       <c r="F19" t="n">
-        <v>2732667152708.93</v>
+        <v>2695649999868.542</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1466,13 +1466,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.5830352112676056</v>
+        <v>0.5844472222222222</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2026586151977836</v>
+        <v>0.201582757598931</v>
       </c>
       <c r="F20" t="n">
-        <v>2842042367972.169</v>
+        <v>2803543461682.486</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1503,13 +1503,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.5911521126760564</v>
+        <v>0.5924361111111112</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1985937438657515</v>
+        <v>0.1974909934159991</v>
       </c>
       <c r="F21" t="n">
-        <v>2951680040124.282</v>
+        <v>2911695646754.444</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1540,13 +1540,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.59363</v>
+        <v>0.5949070422535211</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2014748650846292</v>
+        <v>0.2003198024045863</v>
       </c>
       <c r="F22" t="n">
-        <v>3057450097014.872</v>
+        <v>3015450737405.535</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1577,13 +1577,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.5990420289855073</v>
+        <v>0.6002514285714285</v>
       </c>
       <c r="E23" t="n">
-        <v>0.198616145014771</v>
+        <v>0.1974311090583664</v>
       </c>
       <c r="F23" t="n">
-        <v>3178416529847.667</v>
+        <v>3134127344089.086</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1614,13 +1614,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.4549147959183674</v>
+        <v>0.4553761421319797</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1792837236751567</v>
+        <v>0.178942979714552</v>
       </c>
       <c r="F24" t="n">
-        <v>384536352740.0408</v>
+        <v>382627450533.9797</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1651,13 +1651,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.5981623188405798</v>
+        <v>0.5993814285714285</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2008367255358334</v>
+        <v>0.1996368088484811</v>
       </c>
       <c r="F25" t="n">
-        <v>3288087994260.855</v>
+        <v>3242270509345.543</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1688,13 +1688,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.6001159420289855</v>
+        <v>0.6013128571428572</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1983371450950809</v>
+        <v>0.197149169538422</v>
       </c>
       <c r="F26" t="n">
-        <v>3397721378163.261</v>
+        <v>3350375964397.872</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1725,13 +1725,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.6040768115942029</v>
+        <v>0.6052114285714286</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1980560475819969</v>
+        <v>0.1968446526040247</v>
       </c>
       <c r="F27" t="n">
-        <v>3507526190011.377</v>
+        <v>3458650341187.643</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1762,13 +1762,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.6056420289855072</v>
+        <v>0.6067585714285715</v>
       </c>
       <c r="E28" t="n">
-        <v>0.198599638947155</v>
+        <v>0.1973764493336345</v>
       </c>
       <c r="F28" t="n">
-        <v>3617470476536.102</v>
+        <v>3567062371071.443</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1799,13 +1799,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.6063710144927535</v>
+        <v>0.6074714285714287</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1973265844030929</v>
+        <v>0.1961076975208141</v>
       </c>
       <c r="F29" t="n">
-        <v>3727147406226.522</v>
+        <v>3675210677667.014</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1913,7 +1913,7 @@
         <v>0.6077867647058824</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1949663437502657</v>
+        <v>0.1949663437502658</v>
       </c>
       <c r="F32" t="n">
         <v>3898587515188.338</v>
@@ -1987,7 +1987,7 @@
         <v>0.6106805970149254</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1930700808850805</v>
+        <v>0.1930700808850804</v>
       </c>
       <c r="F34" t="n">
         <v>3468530106897.403</v>
@@ -2021,13 +2021,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.4741370558375634</v>
+        <v>0.4748</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1897267761525686</v>
+        <v>0.1894743980401847</v>
       </c>
       <c r="F35" t="n">
-        <v>531209346349.8883</v>
+        <v>528582781233.1364</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2251,7 +2251,7 @@
         <v>0.6151402985074627</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1897548714268294</v>
+        <v>0.1897548714268295</v>
       </c>
       <c r="F41" t="n">
         <v>4001392447919.433</v>
@@ -2362,7 +2362,7 @@
         <v>0.6196776119402985</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1901408910007902</v>
+        <v>0.1901408910007903</v>
       </c>
       <c r="F44" t="n">
         <v>4268140530208.089</v>
@@ -2433,13 +2433,13 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.6340570852921423</v>
+        <v>0.6340444966442953</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1878002288590449</v>
+        <v>0.1877377846063143</v>
       </c>
       <c r="F46" t="n">
-        <v>578762791544.2616</v>
+        <v>575880487231.8368</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2507,13 +2507,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.486093670886076</v>
+        <v>0.48767625</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1973441685403059</v>
+        <v>0.1966014095547741</v>
       </c>
       <c r="F48" t="n">
-        <v>674386712737.405</v>
+        <v>666163381884.4</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2544,13 +2544,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.5011050632911392</v>
+        <v>0.50261</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2034270983251955</v>
+        <v>0.2025831703557638</v>
       </c>
       <c r="F49" t="n">
-        <v>786679154081.2911</v>
+        <v>777085646997.9</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2581,13 +2581,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.5088746835443038</v>
+        <v>0.51045375</v>
       </c>
       <c r="E50" t="n">
-        <v>0.206412460161286</v>
+        <v>0.2055876017931917</v>
       </c>
       <c r="F50" t="n">
-        <v>927245494005.8228</v>
+        <v>915928457486.2125</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2618,13 +2618,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.5248103896103896</v>
+        <v>0.5264897435897437</v>
       </c>
       <c r="E51" t="n">
-        <v>0.2058806377391979</v>
+        <v>0.2050764162862627</v>
       </c>
       <c r="F51" t="n">
-        <v>990240688644.7533</v>
+        <v>977860226826.1025</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2655,13 +2655,13 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.77711</v>
+        <v>0.7548571428571428</v>
       </c>
       <c r="E52" t="n">
-        <v>0.309537671195105</v>
+        <v>0.3095307135606459</v>
       </c>
       <c r="F52" t="n">
-        <v>154872496903.5</v>
+        <v>131293893808.1429</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2846,7 +2846,7 @@
         <v/>
       </c>
       <c r="F57" t="n">
-        <v>450030999349.2929</v>
+        <v>459992421070.59</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2854,10 +2854,10 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>0.1704422620811848</v>
+        <v>0.1701828594505787</v>
       </c>
       <c r="I57" t="n">
-        <v>0.03696675884396014</v>
+        <v>0.03687094770736327</v>
       </c>
     </row>
     <row r="58">
@@ -2883,7 +2883,7 @@
         <v/>
       </c>
       <c r="F58" t="n">
-        <v>2968583564771.3</v>
+        <v>3997207714061.25</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2891,10 +2891,10 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>0.1861270412802696</v>
+        <v>0.2037849438687166</v>
       </c>
       <c r="I58" t="n">
-        <v>0.07171408386126632</v>
+        <v>0.08730319510038803</v>
       </c>
       <c r="V58" t="inlineStr">
         <is>
@@ -2925,7 +2925,7 @@
         <v/>
       </c>
       <c r="F59" t="n">
-        <v>3265457753721.6</v>
+        <v>4396760286303.667</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2933,10 +2933,10 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>0.1898500710725784</v>
+        <v>0.2086463185648123</v>
       </c>
       <c r="I59" t="n">
-        <v>0.07106446594183173</v>
+        <v>0.08421916776951165</v>
       </c>
     </row>
     <row r="60">
@@ -2962,7 +2962,7 @@
         <v/>
       </c>
       <c r="F60" t="n">
-        <v>3533963251235</v>
+        <v>5020603015415.1</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2970,10 +2970,10 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>0.1759520918130875</v>
+        <v>0.2026146575808525</v>
       </c>
       <c r="I60" t="n">
-        <v>0.06801957307046885</v>
+        <v>0.08972300330629784</v>
       </c>
     </row>
     <row r="61">
@@ -2999,7 +2999,7 @@
         <v/>
       </c>
       <c r="F61" t="n">
-        <v>3828652907036</v>
+        <v>5439664721401.6</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -3007,10 +3007,10 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>0.1765054706484079</v>
+        <v>0.2032675057649612</v>
       </c>
       <c r="I61" t="n">
-        <v>0.07160925999704425</v>
+        <v>0.09844338439459967</v>
       </c>
     </row>
     <row r="62">
@@ -3036,7 +3036,7 @@
         <v/>
       </c>
       <c r="F62" t="n">
-        <v>4122833071393.75</v>
+        <v>5857777920154.3</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -3044,10 +3044,10 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>0.1916059423238039</v>
+        <v>0.2140304088592529</v>
       </c>
       <c r="I62" t="n">
-        <v>0.07428610056954099</v>
+        <v>0.0922283168383857</v>
       </c>
     </row>
     <row r="63">
@@ -3073,7 +3073,7 @@
         <v/>
       </c>
       <c r="F63" t="n">
-        <v>4417558874926.25</v>
+        <v>6276335331130</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -3081,10 +3081,10 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>0.1745931748300791</v>
+        <v>0.2035749703645706</v>
       </c>
       <c r="I63" t="n">
-        <v>0.06774357413870717</v>
+        <v>0.0928362000802636</v>
       </c>
     </row>
     <row r="64">
@@ -3110,7 +3110,7 @@
         <v/>
       </c>
       <c r="F64" t="n">
-        <v>4712407760743.875</v>
+        <v>6695201755220.8</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>0.1728480234742165</v>
+        <v>0.2029298365116119</v>
       </c>
       <c r="I64" t="n">
-        <v>0.06324201895881346</v>
+        <v>0.08847766309646771</v>
       </c>
     </row>
     <row r="65">
@@ -3147,7 +3147,7 @@
         <v/>
       </c>
       <c r="F65" t="n">
-        <v>5006784091093.125</v>
+        <v>7113510849216.9</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -3155,10 +3155,10 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>0.1787202432751656</v>
+        <v>0.2115712642669678</v>
       </c>
       <c r="I65" t="n">
-        <v>0.07144190205365576</v>
+        <v>0.102333081109965</v>
       </c>
     </row>
     <row r="66">
@@ -3184,7 +3184,7 @@
         <v/>
       </c>
       <c r="F66" t="n">
-        <v>5300337760181.75</v>
+        <v>7531455424664.3</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -3192,10 +3192,10 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>0.1772708464413881</v>
+        <v>0.2103892549872398</v>
       </c>
       <c r="I66" t="n">
-        <v>0.07427959868907347</v>
+        <v>0.1016412673812392</v>
       </c>
     </row>
     <row r="67">
@@ -3221,7 +3221,7 @@
         <v/>
       </c>
       <c r="F67" t="n">
-        <v>5595064558115.375</v>
+        <v>7950275760922.4</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -3229,10 +3229,10 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>0.1805790401995182</v>
+        <v>0.212040314078331</v>
       </c>
       <c r="I67" t="n">
-        <v>0.07130951380382484</v>
+        <v>0.0970527111735667</v>
       </c>
     </row>
     <row r="68">
@@ -3258,7 +3258,7 @@
         <v/>
       </c>
       <c r="F68" t="n">
-        <v>902237670536.1034</v>
+        <v>924848220658.5909</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3266,10 +3266,10 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>0.1881771329148062</v>
+        <v>0.1878123955631798</v>
       </c>
       <c r="I68" t="n">
-        <v>0.05503870824255786</v>
+        <v>0.05482834362743141</v>
       </c>
     </row>
     <row r="69">
@@ -3295,7 +3295,7 @@
         <v/>
       </c>
       <c r="F69" t="n">
-        <v>5889667881883.875</v>
+        <v>8368929953138</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3303,10 +3303,10 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>0.1801694761961699</v>
+        <v>0.211614216864109</v>
       </c>
       <c r="I69" t="n">
-        <v>0.07667292930994277</v>
+        <v>0.1016244099877123</v>
       </c>
     </row>
     <row r="70">
@@ -3332,7 +3332,7 @@
         <v/>
       </c>
       <c r="F70" t="n">
-        <v>6182734295294</v>
+        <v>8786353288256.5</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3340,10 +3340,10 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0.1760056354105473</v>
+        <v>0.2098844408988953</v>
       </c>
       <c r="I70" t="n">
-        <v>0.08067729251053302</v>
+        <v>0.1068766156080724</v>
       </c>
     </row>
     <row r="71">
@@ -3369,7 +3369,7 @@
         <v/>
       </c>
       <c r="F71" t="n">
-        <v>6477559698751.125</v>
+        <v>9205105899913</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3377,10 +3377,10 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>0.1758031323552132</v>
+        <v>0.2061373502016068</v>
       </c>
       <c r="I71" t="n">
-        <v>0.07191769812928017</v>
+        <v>0.0921289779237361</v>
       </c>
     </row>
     <row r="72">
@@ -3406,7 +3406,7 @@
         <v/>
       </c>
       <c r="F72" t="n">
-        <v>6771318662562.5</v>
+        <v>9623351270376</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3414,10 +3414,10 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>0.1918547283858061</v>
+        <v>0.220650677382946</v>
       </c>
       <c r="I72" t="n">
-        <v>0.07196120565196328</v>
+        <v>0.09213694000066587</v>
       </c>
     </row>
     <row r="73">
@@ -3443,7 +3443,7 @@
         <v/>
       </c>
       <c r="F73" t="n">
-        <v>7066344752603.5</v>
+        <v>10042714238892.3</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3451,10 +3451,10 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.1882986146956682</v>
+        <v>0.2184548005461693</v>
       </c>
       <c r="I73" t="n">
-        <v>0.07713970785263573</v>
+        <v>0.09894674591903299</v>
       </c>
     </row>
     <row r="74">
@@ -3480,7 +3480,7 @@
         <v/>
       </c>
       <c r="F74" t="n">
-        <v>7360526291942.75</v>
+        <v>10461040614219.5</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3488,10 +3488,10 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>0.1826615128666162</v>
+        <v>0.2161131486296654</v>
       </c>
       <c r="I74" t="n">
-        <v>0.07650291744537038</v>
+        <v>0.1012887900372996</v>
       </c>
     </row>
     <row r="75">
@@ -3517,7 +3517,7 @@
         <v/>
       </c>
       <c r="F75" t="n">
-        <v>7655673648697.5</v>
+        <v>10880022231208.2</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3525,10 +3525,10 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>0.2026659771800041</v>
+        <v>0.235486763715744</v>
       </c>
       <c r="I75" t="n">
-        <v>0.08096076207633401</v>
+        <v>0.1036051754030871</v>
       </c>
     </row>
     <row r="76">
@@ -3554,7 +3554,7 @@
         <v/>
       </c>
       <c r="F76" t="n">
-        <v>7951171910612.25</v>
+        <v>11299395834406.7</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3562,10 +3562,10 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0.1917365342378616</v>
+        <v>0.2251205056905747</v>
       </c>
       <c r="I76" t="n">
-        <v>0.06875768964030336</v>
+        <v>0.0986174158745303</v>
       </c>
     </row>
     <row r="77">
@@ -3591,7 +3591,7 @@
         <v/>
       </c>
       <c r="F77" t="n">
-        <v>8246255078848.5</v>
+        <v>11718271236171</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>0.1811824291944504</v>
+        <v>0.2106122434139252</v>
       </c>
       <c r="I77" t="n">
-        <v>0.07746239955041412</v>
+        <v>0.09805386477381375</v>
       </c>
     </row>
     <row r="78">
@@ -3628,7 +3628,7 @@
         <v/>
       </c>
       <c r="F78" t="n">
-        <v>8540586175314.375</v>
+        <v>12136763324366.9</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3636,10 +3636,10 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.1894466802477837</v>
+        <v>0.220080241560936</v>
       </c>
       <c r="I78" t="n">
-        <v>0.07758982067393008</v>
+        <v>0.09693215036806174</v>
       </c>
     </row>
     <row r="79">
@@ -3665,7 +3665,7 @@
         <v/>
       </c>
       <c r="F79" t="n">
-        <v>1314243230883.869</v>
+        <v>1349820635831.918</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3673,10 +3673,10 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.2001151572025958</v>
+        <v>0.1997351535979439</v>
       </c>
       <c r="I79" t="n">
-        <v>0.06449737283652171</v>
+        <v>0.06420796355944433</v>
       </c>
     </row>
     <row r="80">
@@ -3702,7 +3702,7 @@
         <v/>
       </c>
       <c r="F80" t="n">
-        <v>8835506630048.125</v>
+        <v>12555601432459.1</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3710,10 +3710,10 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>0.1947078965604305</v>
+        <v>0.2248971581459046</v>
       </c>
       <c r="I80" t="n">
-        <v>0.07726817402985407</v>
+        <v>0.09746193562982489</v>
       </c>
     </row>
     <row r="81">
@@ -3739,7 +3739,7 @@
         <v/>
       </c>
       <c r="F81" t="n">
-        <v>9130049005602.75</v>
+        <v>12974289671071.6</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3747,10 +3747,10 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>0.1860596518963575</v>
+        <v>0.2204556182026863</v>
       </c>
       <c r="I81" t="n">
-        <v>0.0751374060370233</v>
+        <v>0.1013762060390661</v>
       </c>
     </row>
     <row r="82">
@@ -3776,7 +3776,7 @@
         <v/>
       </c>
       <c r="F82" t="n">
-        <v>9425610649249.375</v>
+        <v>13393641717959.6</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3784,10 +3784,10 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>0.1834042314440012</v>
+        <v>0.2193862363696098</v>
       </c>
       <c r="I82" t="n">
-        <v>0.07412066476728382</v>
+        <v>0.1028399808264273</v>
       </c>
       <c r="V82" t="inlineStr">
         <is>
@@ -3818,7 +3818,7 @@
         <v/>
       </c>
       <c r="F83" t="n">
-        <v>9720738562145.25</v>
+        <v>13812575690688.7</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3826,10 +3826,10 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>0.1830331943929195</v>
+        <v>0.2147075265645981</v>
       </c>
       <c r="I83" t="n">
-        <v>0.07274024305692223</v>
+        <v>0.09958443762972137</v>
       </c>
     </row>
     <row r="84">
@@ -3855,7 +3855,7 @@
         <v/>
       </c>
       <c r="F84" t="n">
-        <v>10014985168236.88</v>
+        <v>14230950309078.8</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3863,10 +3863,10 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>0.1986057981848717</v>
+        <v>0.2293979346752167</v>
       </c>
       <c r="I84" t="n">
-        <v>0.07809313348605283</v>
+        <v>0.09823523453254365</v>
       </c>
     </row>
     <row r="85">
@@ -3892,7 +3892,7 @@
         <v/>
       </c>
       <c r="F85" t="n">
-        <v>10309757161148.62</v>
+        <v>14649951993276.9</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3900,10 +3900,10 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>0.1833901442587376</v>
+        <v>0.2212859094142914</v>
       </c>
       <c r="I85" t="n">
-        <v>0.07000445209643377</v>
+        <v>0.1032797624421537</v>
       </c>
     </row>
     <row r="86">
@@ -3929,7 +3929,7 @@
         <v/>
       </c>
       <c r="F86" t="n">
-        <v>10604356547791.62</v>
+        <v>15083736264262.6</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3937,10 +3937,10 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>0.2031211648136377</v>
+        <v>0.2363780364394188</v>
       </c>
       <c r="I86" t="n">
-        <v>0.07934894647071287</v>
+        <v>0.1010852169387407</v>
       </c>
     </row>
     <row r="87">
@@ -3966,7 +3966,7 @@
         <v/>
       </c>
       <c r="F87" t="n">
-        <v>10898430868917.88</v>
+        <v>11260895825346.33</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3974,10 +3974,10 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>0.1832808572798967</v>
+        <v>0.2100706415043937</v>
       </c>
       <c r="I87" t="n">
-        <v>0.07320571540825345</v>
+        <v>0.1055861024071628</v>
       </c>
     </row>
     <row r="88">
@@ -4003,7 +4003,7 @@
         <v/>
       </c>
       <c r="F88" t="n">
-        <v>11192850655253.25</v>
+        <v>11565086806375.33</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -4011,10 +4011,10 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>0.2015318423509598</v>
+        <v>0.2219914197921753</v>
       </c>
       <c r="I88" t="n">
-        <v>0.07367139459852201</v>
+        <v>0.09228428287627098</v>
       </c>
     </row>
     <row r="89">
@@ -4040,7 +4040,7 @@
         <v/>
       </c>
       <c r="F89" t="n">
-        <v>11487881847928.25</v>
+        <v>11869946863488.33</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -4048,10 +4048,10 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>0.1930310986936092</v>
+        <v>0.2176889545387692</v>
       </c>
       <c r="I89" t="n">
-        <v>0.06849543101099262</v>
+        <v>0.09786347507949604</v>
       </c>
     </row>
     <row r="90">
@@ -4077,7 +4077,7 @@
         <v/>
       </c>
       <c r="F90" t="n">
-        <v>1745317392389.729</v>
+        <v>1792281688040.477</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -4085,10 +4085,10 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>0.2107047968051013</v>
+        <v>0.2102377187720565</v>
       </c>
       <c r="I90" t="n">
-        <v>0.07820927095547602</v>
+        <v>0.07786842059697734</v>
       </c>
     </row>
     <row r="91">
@@ -4114,7 +4114,7 @@
         <v/>
       </c>
       <c r="F91" t="n">
-        <v>11782250415032.88</v>
+        <v>12174105762849</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -4122,10 +4122,10 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>0.1859051492065191</v>
+        <v>0.2134416417943107</v>
       </c>
       <c r="I91" t="n">
-        <v>0.07266640491454728</v>
+        <v>0.1069798178122482</v>
       </c>
     </row>
     <row r="92">
@@ -4151,7 +4151,7 @@
         <v/>
       </c>
       <c r="F92" t="n">
-        <v>12076338097233.5</v>
+        <v>12478104119725</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -4159,10 +4159,10 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>0.1851323656737804</v>
+        <v>0.2111974391672346</v>
       </c>
       <c r="I92" t="n">
-        <v>0.07388562128693886</v>
+        <v>0.1043608734622792</v>
       </c>
     </row>
     <row r="93">
@@ -4188,7 +4188,7 @@
         <v/>
       </c>
       <c r="F93" t="n">
-        <v>12371093313572.25</v>
+        <v>12782738037802</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -4196,10 +4196,10 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>0.2013100646436214</v>
+        <v>0.225709683365292</v>
       </c>
       <c r="I93" t="n">
-        <v>0.07694136391408077</v>
+        <v>0.1026550015328294</v>
       </c>
     </row>
     <row r="94">
@@ -4225,7 +4225,7 @@
         <v/>
       </c>
       <c r="F94" t="n">
-        <v>12664229246068.62</v>
+        <v>13085816584195.33</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -4233,10 +4233,10 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>0.1888273973017931</v>
+        <v>0.2128185878197352</v>
       </c>
       <c r="I94" t="n">
-        <v>0.07223331889360922</v>
+        <v>0.09872001223562207</v>
       </c>
     </row>
     <row r="95">
@@ -4262,7 +4262,7 @@
         <v/>
       </c>
       <c r="F95" t="n">
-        <v>12959012243525.38</v>
+        <v>13390352748868.55</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -4270,10 +4270,10 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>0.1938723269850016</v>
+        <v>0.219504016968939</v>
       </c>
       <c r="I95" t="n">
-        <v>0.07142377466069931</v>
+        <v>0.1018652930164572</v>
       </c>
     </row>
     <row r="96">
@@ -4299,7 +4299,7 @@
         <v/>
       </c>
       <c r="F96" t="n">
-        <v>13254366729402.88</v>
+        <v>13695505748551.45</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -4307,10 +4307,10 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>0.1829858161509037</v>
+        <v>0.2109212279319763</v>
       </c>
       <c r="I96" t="n">
-        <v>0.07307022546493488</v>
+        <v>0.1081449753835664</v>
       </c>
     </row>
     <row r="97">
@@ -4336,7 +4336,7 @@
         <v/>
       </c>
       <c r="F97" t="n">
-        <v>13549649047011.5</v>
+        <v>14000529518542</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -4344,10 +4344,10 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>0.1999342571943998</v>
+        <v>0.2252375930547714</v>
       </c>
       <c r="I97" t="n">
-        <v>0.07334878742128237</v>
+        <v>0.1023223743377557</v>
       </c>
     </row>
     <row r="98">
@@ -4373,7 +4373,7 @@
         <v/>
       </c>
       <c r="F98" t="n">
-        <v>13884469149822.86</v>
+        <v>14397679048431.25</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -4381,10 +4381,10 @@
         </is>
       </c>
       <c r="H98" t="n">
-        <v>0.187964283994266</v>
+        <v>0.2187952976673841</v>
       </c>
       <c r="I98" t="n">
-        <v>0.07700873921217133</v>
+        <v>0.1126390912355293</v>
       </c>
     </row>
     <row r="99">
@@ -4410,7 +4410,7 @@
         <v/>
       </c>
       <c r="F99" t="n">
-        <v>14180589981977.43</v>
+        <v>14704699205883.62</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -4418,10 +4418,10 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>0.1948428196566445</v>
+        <v>0.217534676194191</v>
       </c>
       <c r="I99" t="n">
-        <v>0.07415046473381895</v>
+        <v>0.09397970016080291</v>
       </c>
     </row>
     <row r="100">
@@ -4447,7 +4447,7 @@
         <v/>
       </c>
       <c r="F100" t="n">
-        <v>14475943991165</v>
+        <v>15010773351995.88</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -4455,10 +4455,10 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>0.1905131680624826</v>
+        <v>0.2212605029344559</v>
       </c>
       <c r="I100" t="n">
-        <v>0.07981155148283595</v>
+        <v>0.1141187503044984</v>
       </c>
     </row>
     <row r="101">
@@ -4484,7 +4484,7 @@
         <v/>
       </c>
       <c r="F101" t="n">
-        <v>2189602599767.786</v>
+        <v>2248899399984.635</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -4492,10 +4492,10 @@
         </is>
       </c>
       <c r="H101" t="n">
-        <v>0.2172274296837194</v>
+        <v>0.216755330211976</v>
       </c>
       <c r="I101" t="n">
-        <v>0.08401351498492113</v>
+        <v>0.08362528499461744</v>
       </c>
     </row>
     <row r="102">
@@ -4521,7 +4521,7 @@
         <v/>
       </c>
       <c r="F102" t="n">
-        <v>14771778885317.57</v>
+        <v>15317779067481.5</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4529,10 +4529,10 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>0.202729657292366</v>
+        <v>0.226020434871316</v>
       </c>
       <c r="I102" t="n">
-        <v>0.07783139757129603</v>
+        <v>0.09763206193254741</v>
       </c>
     </row>
     <row r="103">
@@ -4558,7 +4558,7 @@
         <v/>
       </c>
       <c r="F103" t="n">
-        <v>1828109571803.636</v>
+        <v>2398735748890.25</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4566,10 +4566,10 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>0.1827357126907869</v>
+        <v>0.183305108298858</v>
       </c>
       <c r="I103" t="n">
-        <v>0.06490658907691857</v>
+        <v>0.06191742958850368</v>
       </c>
     </row>
     <row r="104">
@@ -4595,7 +4595,7 @@
         <v/>
       </c>
       <c r="F104" t="n">
-        <v>2132214648603.455</v>
+        <v>2798004037576.25</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4603,10 +4603,10 @@
         </is>
       </c>
       <c r="H104" t="n">
-        <v>0.1869625300168991</v>
+        <v>0.1882850701610247</v>
       </c>
       <c r="I104" t="n">
-        <v>0.07385404112544985</v>
+        <v>0.07056594385056314</v>
       </c>
     </row>
     <row r="105">
@@ -4632,7 +4632,7 @@
         <v/>
       </c>
       <c r="F105" t="n">
-        <v>2436959358794.455</v>
+        <v>3197894582411.417</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4640,10 +4640,10 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>0.1852527436884967</v>
+        <v>0.1870441511273384</v>
       </c>
       <c r="I105" t="n">
-        <v>0.08030021051221893</v>
+        <v>0.07681432432930396</v>
       </c>
     </row>
     <row r="106">
@@ -4669,7 +4669,7 @@
         <v/>
       </c>
       <c r="F106" t="n">
-        <v>2671802437954</v>
+        <v>3597584389032.583</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4677,10 +4677,10 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>0.1611605532467365</v>
+        <v>0.1821188113341729</v>
       </c>
       <c r="I106" t="n">
-        <v>0.06760391955079546</v>
+        <v>0.08444873575037527</v>
       </c>
       <c r="V106" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
sorted epoch to int for proper handling and added some spaces to among epoch better visualization in plots
</commit_message>
<xml_diff>
--- a/excel/statistics.xlsx
+++ b/excel/statistics.xlsx
@@ -789,19 +789,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C2" t="n">
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3956729515828677</v>
+        <v>0.395702515137401</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1406268584264503</v>
+        <v>0.1406529428055432</v>
       </c>
       <c r="F2" t="n">
-        <v>141645697853.1395</v>
+        <v>141863172318.9341</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -826,19 +824,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="C3" t="n">
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5257717948717948</v>
+        <v>0.5230260133091349</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2060228312259274</v>
+        <v>0.1613087964420446</v>
       </c>
       <c r="F3" t="n">
-        <v>1113584289929.833</v>
+        <v>281706336983.4059</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -863,19 +859,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="C4" t="n">
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5323763157894736</v>
+        <v>0.4549147959183674</v>
       </c>
       <c r="E4" t="n">
-        <v>0.200923416168729</v>
+        <v>0.1792837236751567</v>
       </c>
       <c r="F4" t="n">
-        <v>1205503821556.079</v>
+        <v>384536352740.0408</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -900,19 +894,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="C5" t="n">
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5377090909090909</v>
+        <v>0.4741370558375634</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2062981823668035</v>
+        <v>0.1897267761525686</v>
       </c>
       <c r="F5" t="n">
-        <v>1342287262533.286</v>
+        <v>531209346349.8883</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -937,19 +929,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="C6" t="n">
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5482907894736841</v>
+        <v>0.6340570852921423</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1976738554134944</v>
+        <v>0.1878002288590449</v>
       </c>
       <c r="F6" t="n">
-        <v>1424792523738.25</v>
+        <v>578762791544.2616</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -974,19 +964,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="C7" t="n">
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5465671052631579</v>
+        <v>0.486093670886076</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2036673067451969</v>
+        <v>0.1973441685403059</v>
       </c>
       <c r="F7" t="n">
-        <v>1562831919165.171</v>
+        <v>674386712737.405</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1011,19 +999,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="C8" t="n">
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5459506666666667</v>
+        <v>0.5011050632911392</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2064819234109743</v>
+        <v>0.2034270983251955</v>
       </c>
       <c r="F8" t="n">
-        <v>1617033360696.32</v>
+        <v>786679154081.2911</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1048,19 +1034,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="C9" t="n">
+        <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5568960000000001</v>
+        <v>0.5088746835443038</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2057089622402143</v>
+        <v>0.206412460161286</v>
       </c>
       <c r="F9" t="n">
-        <v>1724946791383.813</v>
+        <v>927245494005.8228</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1085,19 +1069,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="C10" t="n">
+        <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5616594594594595</v>
+        <v>0.5248103896103896</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1997064838802521</v>
+        <v>0.2058806377391979</v>
       </c>
       <c r="F10" t="n">
-        <v>1836514193219.297</v>
+        <v>990240688644.7533</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1122,19 +1104,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="C11" t="n">
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5639378378378378</v>
+        <v>0.5238194805194805</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2015745673936039</v>
+        <v>0.2066462869373407</v>
       </c>
       <c r="F11" t="n">
-        <v>1944573126475.581</v>
+        <v>1127692693324.948</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1159,19 +1139,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C12" t="n">
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5690986486486487</v>
+        <v>0.53038</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2026503740626646</v>
+        <v>0.2015162242814426</v>
       </c>
       <c r="F12" t="n">
-        <v>2052717496138.013</v>
+        <v>1221178546075.347</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1196,19 +1174,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C13" t="n">
+        <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5230296856106409</v>
+        <v>0.5357776315789473</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1612600654810651</v>
+        <v>0.2069669330102012</v>
       </c>
       <c r="F13" t="n">
-        <v>280347162297.0295</v>
+        <v>1359519905000.921</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1233,19 +1209,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="C14" t="n">
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5739716216216216</v>
+        <v>0.5464760000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2033843116484937</v>
+        <v>0.1983665988122101</v>
       </c>
       <c r="F14" t="n">
-        <v>2160909321594.906</v>
+        <v>1443319379853.133</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1270,19 +1244,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="C15" t="n">
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5772716216216216</v>
+        <v>0.5447386666666667</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2001354688603808</v>
+        <v>0.2044098862403499</v>
       </c>
       <c r="F15" t="n">
-        <v>2269401210093.243</v>
+        <v>1583163532589.2</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1307,19 +1279,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="C16" t="n">
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5771333333333334</v>
+        <v>0.5440891891891891</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2023248406072783</v>
+        <v>0.207256798270818</v>
       </c>
       <c r="F16" t="n">
-        <v>2371383336712.25</v>
+        <v>1638335764204.432</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1344,19 +1314,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="C17" t="n">
+        <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5777222222222222</v>
+        <v>0.5551797297297297</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2039693750985445</v>
+        <v>0.2065717932048593</v>
       </c>
       <c r="F17" t="n">
-        <v>2479517378536.597</v>
+        <v>1747671191657.513</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1381,19 +1349,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="C18" t="n">
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5830319444444444</v>
+        <v>0.5599808219178082</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2052782253680366</v>
+        <v>0.2005621867107654</v>
       </c>
       <c r="F18" t="n">
-        <v>2587709937089.431</v>
+        <v>1861041395419.712</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1418,19 +1384,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="C19" t="n">
+        <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5859319444444444</v>
+        <v>0.5622739726027397</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1991416466840957</v>
+        <v>0.202457238302175</v>
       </c>
       <c r="F19" t="n">
-        <v>2695649999868.542</v>
+        <v>1970544057279.548</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1460,19 +1424,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="C20" t="n">
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5844472222222222</v>
+        <v>0.5675287671232877</v>
       </c>
       <c r="E20" t="n">
-        <v>0.201582757598931</v>
+        <v>0.2035992226569504</v>
       </c>
       <c r="F20" t="n">
-        <v>2803543461682.486</v>
+        <v>2080133082254.069</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1497,19 +1459,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="C21" t="n">
+        <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5924361111111112</v>
+        <v>0.5724684931506849</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1974909934159991</v>
+        <v>0.2043775359181523</v>
       </c>
       <c r="F21" t="n">
-        <v>2911695646754.444</v>
+        <v>2189770455562.274</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1534,19 +1494,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="C22" t="n">
+        <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5949070422535211</v>
+        <v>0.5758109589041096</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2003198024045863</v>
+        <v>0.2011229471697211</v>
       </c>
       <c r="F22" t="n">
-        <v>3015450737405.535</v>
+        <v>2299711902643.822</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1571,19 +1529,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="C23" t="n">
+        <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6002514285714285</v>
+        <v>0.5756323943661972</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1974311090583664</v>
+        <v>0.203360791820595</v>
       </c>
       <c r="F23" t="n">
-        <v>3134127344089.086</v>
+        <v>2403946219823.422</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1608,19 +1564,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C24" t="n">
+        <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4553761421319797</v>
+        <v>0.5762295774647888</v>
       </c>
       <c r="E24" t="n">
-        <v>0.178942979714552</v>
+        <v>0.205024717948395</v>
       </c>
       <c r="F24" t="n">
-        <v>382627450533.9797</v>
+        <v>2513565414321.338</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1645,19 +1599,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="C25" t="n">
+        <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5993814285714285</v>
+        <v>0.5816225352112676</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1996368088484811</v>
+        <v>0.2063881566350045</v>
       </c>
       <c r="F25" t="n">
-        <v>3242270509345.543</v>
+        <v>2623244229421.845</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1682,19 +1634,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="C26" t="n">
+        <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6013128571428572</v>
+        <v>0.5845464788732394</v>
       </c>
       <c r="E26" t="n">
-        <v>0.197149169538422</v>
+        <v>0.2002092661127965</v>
       </c>
       <c r="F26" t="n">
-        <v>3350375964397.872</v>
+        <v>2732667152708.93</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1719,19 +1669,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="C27" t="n">
+        <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.6052114285714286</v>
+        <v>0.5830352112676056</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1968446526040247</v>
+        <v>0.2026586151977836</v>
       </c>
       <c r="F27" t="n">
-        <v>3458650341187.643</v>
+        <v>2842042367972.169</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1756,19 +1704,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="C28" t="n">
+        <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6067585714285715</v>
+        <v>0.5911521126760564</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1973764493336345</v>
+        <v>0.1985937438657515</v>
       </c>
       <c r="F28" t="n">
-        <v>3567062371071.443</v>
+        <v>2951680040124.282</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1793,19 +1739,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="C29" t="n">
+        <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6074714285714287</v>
+        <v>0.59363</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1961076975208141</v>
+        <v>0.2014748650846292</v>
       </c>
       <c r="F29" t="n">
-        <v>3675210677667.014</v>
+        <v>3057450097014.872</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1830,19 +1774,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="C30" t="n">
+        <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6035955882352941</v>
+        <v>0.5990420289855073</v>
       </c>
       <c r="E30" t="n">
-        <v>0.195601171618308</v>
+        <v>0.198616145014771</v>
       </c>
       <c r="F30" t="n">
-        <v>3687795850945.529</v>
+        <v>3178416529847.667</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1867,19 +1809,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="C31" t="n">
+        <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6045867647058824</v>
+        <v>0.5981623188405798</v>
       </c>
       <c r="E31" t="n">
-        <v>0.194410256243492</v>
+        <v>0.2008367255358334</v>
       </c>
       <c r="F31" t="n">
-        <v>3793148879566.191</v>
+        <v>3288087994260.855</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1904,19 +1844,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="C32" t="n">
+        <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6077867647058824</v>
+        <v>0.6001159420289855</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1949663437502658</v>
+        <v>0.1983371450950809</v>
       </c>
       <c r="F32" t="n">
-        <v>3898587515188.338</v>
+        <v>3397721378163.261</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1941,19 +1879,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C33" t="n">
+        <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.606185294117647</v>
+        <v>0.6040768115942029</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1942045054311639</v>
+        <v>0.1980560475819969</v>
       </c>
       <c r="F33" t="n">
-        <v>4003947365611.162</v>
+        <v>3507526190011.377</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1978,19 +1914,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="C34" t="n">
+        <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>0.6106805970149254</v>
+        <v>0.6056420289855072</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1930700808850804</v>
+        <v>0.198599638947155</v>
       </c>
       <c r="F34" t="n">
-        <v>3468530106897.403</v>
+        <v>3617470476536.102</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2015,19 +1949,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C35" t="n">
+        <v>34</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4748</v>
+        <v>0.6063710144927535</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1894743980401847</v>
+        <v>0.1973265844030929</v>
       </c>
       <c r="F35" t="n">
-        <v>528582781233.1364</v>
+        <v>3727147406226.522</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2052,19 +1984,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="C36" t="n">
+        <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>0.6130089552238807</v>
+        <v>0.6035955882352941</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1946008391175525</v>
+        <v>0.195601171618308</v>
       </c>
       <c r="F36" t="n">
-        <v>3557208080952.522</v>
+        <v>3687795850945.529</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2089,19 +2019,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="C37" t="n">
+        <v>36</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6172611940298507</v>
+        <v>0.6045867647058824</v>
       </c>
       <c r="E37" t="n">
-        <v>0.192883019937917</v>
+        <v>0.194410256243492</v>
       </c>
       <c r="F37" t="n">
-        <v>3646145856666.925</v>
+        <v>3793148879566.191</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2131,19 +2059,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="C38" t="n">
+        <v>37</v>
       </c>
       <c r="D38" t="n">
-        <v>0.612341791044776</v>
+        <v>0.6077867647058824</v>
       </c>
       <c r="E38" t="n">
-        <v>0.194068369044031</v>
+        <v>0.1949663437502657</v>
       </c>
       <c r="F38" t="n">
-        <v>3735178105362.179</v>
+        <v>3898587515188.338</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2168,19 +2094,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="C39" t="n">
+        <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6149402985074627</v>
+        <v>0.606185294117647</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1930936780501626</v>
+        <v>0.1942045054311639</v>
       </c>
       <c r="F39" t="n">
-        <v>3823884921871.985</v>
+        <v>4003947365611.162</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2205,19 +2129,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="C40" t="n">
+        <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>0.614120895522388</v>
+        <v>0.6106805970149254</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1920223223587153</v>
+        <v>0.1930700808850805</v>
       </c>
       <c r="F40" t="n">
-        <v>3912680876316.925</v>
+        <v>3468530106897.403</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2242,19 +2164,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C41" t="n">
+        <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>0.6151402985074627</v>
+        <v>0.6130089552238807</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1897548714268295</v>
+        <v>0.1946008391175525</v>
       </c>
       <c r="F41" t="n">
-        <v>4001392447919.433</v>
+        <v>3557208080952.522</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2279,19 +2199,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
+      <c r="C42" t="n">
+        <v>41</v>
       </c>
       <c r="D42" t="n">
-        <v>0.6173223880597014</v>
+        <v>0.6172611940298507</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1898599753733162</v>
+        <v>0.192883019937917</v>
       </c>
       <c r="F42" t="n">
-        <v>4090261830884.493</v>
+        <v>3646145856666.925</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2316,19 +2234,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="C43" t="n">
+        <v>42</v>
       </c>
       <c r="D43" t="n">
-        <v>0.6184388059701492</v>
+        <v>0.612341791044776</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1922325280354923</v>
+        <v>0.194068369044031</v>
       </c>
       <c r="F43" t="n">
-        <v>4179177438112.612</v>
+        <v>3735178105362.179</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2353,19 +2269,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="C44" t="n">
+        <v>43</v>
       </c>
       <c r="D44" t="n">
-        <v>0.6196776119402985</v>
+        <v>0.6149402985074627</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1901408910007903</v>
+        <v>0.1930936780501626</v>
       </c>
       <c r="F44" t="n">
-        <v>4268140530208.089</v>
+        <v>3823884921871.985</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2390,19 +2304,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="C45" t="n">
+        <v>44</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6212089552238806</v>
+        <v>0.614120895522388</v>
       </c>
       <c r="E45" t="n">
-        <v>0.191924786981731</v>
+        <v>0.1920223223587153</v>
       </c>
       <c r="F45" t="n">
-        <v>4357217364261.552</v>
+        <v>3912680876316.925</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2427,19 +2339,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C46" t="n">
+        <v>45</v>
       </c>
       <c r="D46" t="n">
-        <v>0.6340444966442953</v>
+        <v>0.6151402985074627</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1877377846063143</v>
+        <v>0.1897548714268294</v>
       </c>
       <c r="F46" t="n">
-        <v>575880487231.8368</v>
+        <v>4001392447919.433</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2464,19 +2374,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="C47" t="n">
+        <v>46</v>
       </c>
       <c r="D47" t="n">
-        <v>0.6225373134328358</v>
+        <v>0.6173223880597014</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1921749091526376</v>
+        <v>0.1898599753733162</v>
       </c>
       <c r="F47" t="n">
-        <v>4445962670216.09</v>
+        <v>4090261830884.493</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2501,19 +2409,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="C48" t="n">
+        <v>47</v>
       </c>
       <c r="D48" t="n">
-        <v>0.48767625</v>
+        <v>0.6184388059701492</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1966014095547741</v>
+        <v>0.1922325280354923</v>
       </c>
       <c r="F48" t="n">
-        <v>666163381884.4</v>
+        <v>4179177438112.612</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2538,19 +2444,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C49" t="n">
+        <v>48</v>
       </c>
       <c r="D49" t="n">
-        <v>0.50261</v>
+        <v>0.6196776119402985</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2025831703557638</v>
+        <v>0.1901408910007902</v>
       </c>
       <c r="F49" t="n">
-        <v>777085646997.9</v>
+        <v>4268140530208.089</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2575,19 +2479,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="C50" t="n">
+        <v>49</v>
       </c>
       <c r="D50" t="n">
-        <v>0.51045375</v>
+        <v>0.6212089552238806</v>
       </c>
       <c r="E50" t="n">
-        <v>0.2055876017931917</v>
+        <v>0.191924786981731</v>
       </c>
       <c r="F50" t="n">
-        <v>915928457486.2125</v>
+        <v>4357217364261.552</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2612,19 +2514,17 @@
           <t>cifar-10</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C51" t="n">
+        <v>50</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5264897435897437</v>
+        <v>0.6225373134328358</v>
       </c>
       <c r="E51" t="n">
-        <v>0.2050764162862627</v>
+        <v>0.1921749091526376</v>
       </c>
       <c r="F51" t="n">
-        <v>977860226826.1025</v>
+        <v>4445962670216.09</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2649,19 +2549,17 @@
           <t>mnist</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C52" t="n">
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7548571428571428</v>
+        <v>0.77711</v>
       </c>
       <c r="E52" t="n">
-        <v>0.3095307135606459</v>
+        <v>0.309537671195105</v>
       </c>
       <c r="F52" t="n">
-        <v>131293893808.1429</v>
+        <v>154872496903.5</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2686,10 +2584,8 @@
           <t>mnist</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C53" t="n">
+        <v>2</v>
       </c>
       <c r="D53" t="n">
         <v>0.911675</v>
@@ -2723,10 +2619,8 @@
           <t>mnist</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C54" t="n">
+        <v>3</v>
       </c>
       <c r="D54" t="n">
         <v>0.9298125</v>
@@ -2760,10 +2654,8 @@
           <t>mnist</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C55" t="n">
+        <v>4</v>
       </c>
       <c r="D55" t="n">
         <v>0.9244875</v>
@@ -2797,10 +2689,8 @@
           <t>mnist</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C56" t="n">
+        <v>5</v>
       </c>
       <c r="D56" t="n">
         <v>0.9813571428571429</v>
@@ -2834,10 +2724,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C57" t="n">
+        <v>1</v>
       </c>
       <c r="D57" t="n">
         <v/>
@@ -2846,7 +2734,7 @@
         <v/>
       </c>
       <c r="F57" t="n">
-        <v>459992421070.59</v>
+        <v>450030999349.2929</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2854,10 +2742,10 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>0.1701828594505787</v>
+        <v>0.1704422620811848</v>
       </c>
       <c r="I57" t="n">
-        <v>0.03687094770736327</v>
+        <v>0.03696675884396014</v>
       </c>
     </row>
     <row r="58">
@@ -2871,10 +2759,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="C58" t="n">
+        <v>2</v>
       </c>
       <c r="D58" t="n">
         <v/>
@@ -2883,7 +2769,7 @@
         <v/>
       </c>
       <c r="F58" t="n">
-        <v>3997207714061.25</v>
+        <v>902237670536.1034</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2891,10 +2777,10 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>0.2037849438687166</v>
+        <v>0.1881771329148062</v>
       </c>
       <c r="I58" t="n">
-        <v>0.08730319510038803</v>
+        <v>0.05503870824255786</v>
       </c>
       <c r="V58" t="inlineStr">
         <is>
@@ -2913,10 +2799,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="C59" t="n">
+        <v>3</v>
       </c>
       <c r="D59" t="n">
         <v/>
@@ -2925,7 +2809,7 @@
         <v/>
       </c>
       <c r="F59" t="n">
-        <v>4396760286303.667</v>
+        <v>1314243230883.869</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2933,10 +2817,10 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>0.2086463185648123</v>
+        <v>0.2001151572025958</v>
       </c>
       <c r="I59" t="n">
-        <v>0.08421916776951165</v>
+        <v>0.06449737283652171</v>
       </c>
     </row>
     <row r="60">
@@ -2950,10 +2834,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="C60" t="n">
+        <v>4</v>
       </c>
       <c r="D60" t="n">
         <v/>
@@ -2962,7 +2844,7 @@
         <v/>
       </c>
       <c r="F60" t="n">
-        <v>5020603015415.1</v>
+        <v>1745317392389.729</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2970,10 +2852,10 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>0.2026146575808525</v>
+        <v>0.2107047968051013</v>
       </c>
       <c r="I60" t="n">
-        <v>0.08972300330629784</v>
+        <v>0.07820927095547602</v>
       </c>
     </row>
     <row r="61">
@@ -2987,10 +2869,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="C61" t="n">
+        <v>5</v>
       </c>
       <c r="D61" t="n">
         <v/>
@@ -2999,7 +2879,7 @@
         <v/>
       </c>
       <c r="F61" t="n">
-        <v>5439664721401.6</v>
+        <v>2189602599767.786</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -3007,10 +2887,10 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>0.2032675057649612</v>
+        <v>0.2172274296837194</v>
       </c>
       <c r="I61" t="n">
-        <v>0.09844338439459967</v>
+        <v>0.08401351498492113</v>
       </c>
     </row>
     <row r="62">
@@ -3024,10 +2904,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="C62" t="n">
+        <v>6</v>
       </c>
       <c r="D62" t="n">
         <v/>
@@ -3036,7 +2914,7 @@
         <v/>
       </c>
       <c r="F62" t="n">
-        <v>5857777920154.3</v>
+        <v>1828109571803.636</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -3044,10 +2922,10 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>0.2140304088592529</v>
+        <v>0.1827357126907869</v>
       </c>
       <c r="I62" t="n">
-        <v>0.0922283168383857</v>
+        <v>0.06490658907691857</v>
       </c>
     </row>
     <row r="63">
@@ -3061,10 +2939,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="C63" t="n">
+        <v>7</v>
       </c>
       <c r="D63" t="n">
         <v/>
@@ -3073,7 +2949,7 @@
         <v/>
       </c>
       <c r="F63" t="n">
-        <v>6276335331130</v>
+        <v>2132214648603.455</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -3081,10 +2957,10 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>0.2035749703645706</v>
+        <v>0.1869625300168991</v>
       </c>
       <c r="I63" t="n">
-        <v>0.0928362000802636</v>
+        <v>0.07385404112544985</v>
       </c>
     </row>
     <row r="64">
@@ -3098,10 +2974,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="C64" t="n">
+        <v>8</v>
       </c>
       <c r="D64" t="n">
         <v/>
@@ -3110,7 +2984,7 @@
         <v/>
       </c>
       <c r="F64" t="n">
-        <v>6695201755220.8</v>
+        <v>2436959358794.455</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3118,10 +2992,10 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>0.2029298365116119</v>
+        <v>0.1852527436884967</v>
       </c>
       <c r="I64" t="n">
-        <v>0.08847766309646771</v>
+        <v>0.08030021051221893</v>
       </c>
     </row>
     <row r="65">
@@ -3135,10 +3009,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="C65" t="n">
+        <v>9</v>
       </c>
       <c r="D65" t="n">
         <v/>
@@ -3147,7 +3019,7 @@
         <v/>
       </c>
       <c r="F65" t="n">
-        <v>7113510849216.9</v>
+        <v>2671802437954</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -3155,10 +3027,10 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>0.2115712642669678</v>
+        <v>0.1611605532467365</v>
       </c>
       <c r="I65" t="n">
-        <v>0.102333081109965</v>
+        <v>0.06760391955079546</v>
       </c>
     </row>
     <row r="66">
@@ -3172,10 +3044,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="C66" t="n">
+        <v>10</v>
       </c>
       <c r="D66" t="n">
         <v/>
@@ -3184,7 +3054,7 @@
         <v/>
       </c>
       <c r="F66" t="n">
-        <v>7531455424664.3</v>
+        <v>2968583564771.3</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -3192,10 +3062,10 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>0.2103892549872398</v>
+        <v>0.1861270412802696</v>
       </c>
       <c r="I66" t="n">
-        <v>0.1016412673812392</v>
+        <v>0.07171408386126632</v>
       </c>
     </row>
     <row r="67">
@@ -3209,10 +3079,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C67" t="n">
+        <v>11</v>
       </c>
       <c r="D67" t="n">
         <v/>
@@ -3221,7 +3089,7 @@
         <v/>
       </c>
       <c r="F67" t="n">
-        <v>7950275760922.4</v>
+        <v>3265457753721.6</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -3229,10 +3097,10 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>0.212040314078331</v>
+        <v>0.1898500710725784</v>
       </c>
       <c r="I67" t="n">
-        <v>0.0970527111735667</v>
+        <v>0.07106446594183173</v>
       </c>
     </row>
     <row r="68">
@@ -3246,10 +3114,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C68" t="n">
+        <v>12</v>
       </c>
       <c r="D68" t="n">
         <v/>
@@ -3258,7 +3124,7 @@
         <v/>
       </c>
       <c r="F68" t="n">
-        <v>924848220658.5909</v>
+        <v>3533963251235</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3266,10 +3132,10 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>0.1878123955631798</v>
+        <v>0.1759520918130875</v>
       </c>
       <c r="I68" t="n">
-        <v>0.05482834362743141</v>
+        <v>0.06801957307046885</v>
       </c>
     </row>
     <row r="69">
@@ -3283,10 +3149,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="C69" t="n">
+        <v>13</v>
       </c>
       <c r="D69" t="n">
         <v/>
@@ -3295,7 +3159,7 @@
         <v/>
       </c>
       <c r="F69" t="n">
-        <v>8368929953138</v>
+        <v>3828652907036</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3303,10 +3167,10 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>0.211614216864109</v>
+        <v>0.1765054706484079</v>
       </c>
       <c r="I69" t="n">
-        <v>0.1016244099877123</v>
+        <v>0.07160925999704425</v>
       </c>
     </row>
     <row r="70">
@@ -3320,10 +3184,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="C70" t="n">
+        <v>14</v>
       </c>
       <c r="D70" t="n">
         <v/>
@@ -3332,7 +3194,7 @@
         <v/>
       </c>
       <c r="F70" t="n">
-        <v>8786353288256.5</v>
+        <v>4122833071393.75</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3340,10 +3202,10 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0.2098844408988953</v>
+        <v>0.1916059423238039</v>
       </c>
       <c r="I70" t="n">
-        <v>0.1068766156080724</v>
+        <v>0.07428610056954099</v>
       </c>
     </row>
     <row r="71">
@@ -3357,10 +3219,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="C71" t="n">
+        <v>15</v>
       </c>
       <c r="D71" t="n">
         <v/>
@@ -3369,7 +3229,7 @@
         <v/>
       </c>
       <c r="F71" t="n">
-        <v>9205105899913</v>
+        <v>4417558874926.25</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3377,10 +3237,10 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>0.2061373502016068</v>
+        <v>0.1745931748300791</v>
       </c>
       <c r="I71" t="n">
-        <v>0.0921289779237361</v>
+        <v>0.06774357413870717</v>
       </c>
     </row>
     <row r="72">
@@ -3394,10 +3254,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="C72" t="n">
+        <v>16</v>
       </c>
       <c r="D72" t="n">
         <v/>
@@ -3406,7 +3264,7 @@
         <v/>
       </c>
       <c r="F72" t="n">
-        <v>9623351270376</v>
+        <v>4712407760743.875</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3414,10 +3272,10 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>0.220650677382946</v>
+        <v>0.1728480234742165</v>
       </c>
       <c r="I72" t="n">
-        <v>0.09213694000066587</v>
+        <v>0.06324201895881346</v>
       </c>
     </row>
     <row r="73">
@@ -3431,10 +3289,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="C73" t="n">
+        <v>17</v>
       </c>
       <c r="D73" t="n">
         <v/>
@@ -3443,7 +3299,7 @@
         <v/>
       </c>
       <c r="F73" t="n">
-        <v>10042714238892.3</v>
+        <v>5006784091093.125</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3451,10 +3307,10 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.2184548005461693</v>
+        <v>0.1787202432751656</v>
       </c>
       <c r="I73" t="n">
-        <v>0.09894674591903299</v>
+        <v>0.07144190205365576</v>
       </c>
     </row>
     <row r="74">
@@ -3468,10 +3324,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="C74" t="n">
+        <v>18</v>
       </c>
       <c r="D74" t="n">
         <v/>
@@ -3480,7 +3334,7 @@
         <v/>
       </c>
       <c r="F74" t="n">
-        <v>10461040614219.5</v>
+        <v>5300337760181.75</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3488,10 +3342,10 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>0.2161131486296654</v>
+        <v>0.1772708464413881</v>
       </c>
       <c r="I74" t="n">
-        <v>0.1012887900372996</v>
+        <v>0.07427959868907347</v>
       </c>
     </row>
     <row r="75">
@@ -3505,10 +3359,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="C75" t="n">
+        <v>19</v>
       </c>
       <c r="D75" t="n">
         <v/>
@@ -3517,7 +3369,7 @@
         <v/>
       </c>
       <c r="F75" t="n">
-        <v>10880022231208.2</v>
+        <v>5595064558115.375</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3525,10 +3377,10 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>0.235486763715744</v>
+        <v>0.1805790401995182</v>
       </c>
       <c r="I75" t="n">
-        <v>0.1036051754030871</v>
+        <v>0.07130951380382484</v>
       </c>
     </row>
     <row r="76">
@@ -3542,10 +3394,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="C76" t="n">
+        <v>20</v>
       </c>
       <c r="D76" t="n">
         <v/>
@@ -3554,7 +3404,7 @@
         <v/>
       </c>
       <c r="F76" t="n">
-        <v>11299395834406.7</v>
+        <v>5889667881883.875</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3562,10 +3412,10 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0.2251205056905747</v>
+        <v>0.1801694761961699</v>
       </c>
       <c r="I76" t="n">
-        <v>0.0986174158745303</v>
+        <v>0.07667292930994277</v>
       </c>
     </row>
     <row r="77">
@@ -3579,10 +3429,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="C77" t="n">
+        <v>21</v>
       </c>
       <c r="D77" t="n">
         <v/>
@@ -3591,7 +3439,7 @@
         <v/>
       </c>
       <c r="F77" t="n">
-        <v>11718271236171</v>
+        <v>6182734295294</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3599,10 +3447,10 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>0.2106122434139252</v>
+        <v>0.1760056354105473</v>
       </c>
       <c r="I77" t="n">
-        <v>0.09805386477381375</v>
+        <v>0.08067729251053302</v>
       </c>
     </row>
     <row r="78">
@@ -3616,10 +3464,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="C78" t="n">
+        <v>22</v>
       </c>
       <c r="D78" t="n">
         <v/>
@@ -3628,7 +3474,7 @@
         <v/>
       </c>
       <c r="F78" t="n">
-        <v>12136763324366.9</v>
+        <v>6477559698751.125</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3636,10 +3482,10 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.220080241560936</v>
+        <v>0.1758031323552132</v>
       </c>
       <c r="I78" t="n">
-        <v>0.09693215036806174</v>
+        <v>0.07191769812928017</v>
       </c>
     </row>
     <row r="79">
@@ -3653,10 +3499,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C79" t="n">
+        <v>23</v>
       </c>
       <c r="D79" t="n">
         <v/>
@@ -3665,7 +3509,7 @@
         <v/>
       </c>
       <c r="F79" t="n">
-        <v>1349820635831.918</v>
+        <v>6771318662562.5</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3673,10 +3517,10 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.1997351535979439</v>
+        <v>0.1918547283858061</v>
       </c>
       <c r="I79" t="n">
-        <v>0.06420796355944433</v>
+        <v>0.07196120565196328</v>
       </c>
     </row>
     <row r="80">
@@ -3690,10 +3534,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="C80" t="n">
+        <v>24</v>
       </c>
       <c r="D80" t="n">
         <v/>
@@ -3702,7 +3544,7 @@
         <v/>
       </c>
       <c r="F80" t="n">
-        <v>12555601432459.1</v>
+        <v>7066344752603.5</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3710,10 +3552,10 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>0.2248971581459046</v>
+        <v>0.1882986146956682</v>
       </c>
       <c r="I80" t="n">
-        <v>0.09746193562982489</v>
+        <v>0.07713970785263573</v>
       </c>
     </row>
     <row r="81">
@@ -3727,10 +3569,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="C81" t="n">
+        <v>25</v>
       </c>
       <c r="D81" t="n">
         <v/>
@@ -3739,7 +3579,7 @@
         <v/>
       </c>
       <c r="F81" t="n">
-        <v>12974289671071.6</v>
+        <v>7360526291942.75</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3747,10 +3587,10 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>0.2204556182026863</v>
+        <v>0.1826615128666162</v>
       </c>
       <c r="I81" t="n">
-        <v>0.1013762060390661</v>
+        <v>0.07650291744537038</v>
       </c>
     </row>
     <row r="82">
@@ -3764,10 +3604,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="C82" t="n">
+        <v>26</v>
       </c>
       <c r="D82" t="n">
         <v/>
@@ -3776,7 +3614,7 @@
         <v/>
       </c>
       <c r="F82" t="n">
-        <v>13393641717959.6</v>
+        <v>7655673648697.5</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3784,10 +3622,10 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>0.2193862363696098</v>
+        <v>0.2026659771800041</v>
       </c>
       <c r="I82" t="n">
-        <v>0.1028399808264273</v>
+        <v>0.08096076207633401</v>
       </c>
       <c r="V82" t="inlineStr">
         <is>
@@ -3806,10 +3644,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="C83" t="n">
+        <v>27</v>
       </c>
       <c r="D83" t="n">
         <v/>
@@ -3818,7 +3654,7 @@
         <v/>
       </c>
       <c r="F83" t="n">
-        <v>13812575690688.7</v>
+        <v>7951171910612.25</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3826,10 +3662,10 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>0.2147075265645981</v>
+        <v>0.1917365342378616</v>
       </c>
       <c r="I83" t="n">
-        <v>0.09958443762972137</v>
+        <v>0.06875768964030336</v>
       </c>
     </row>
     <row r="84">
@@ -3843,10 +3679,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="C84" t="n">
+        <v>28</v>
       </c>
       <c r="D84" t="n">
         <v/>
@@ -3855,7 +3689,7 @@
         <v/>
       </c>
       <c r="F84" t="n">
-        <v>14230950309078.8</v>
+        <v>8246255078848.5</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3863,10 +3697,10 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>0.2293979346752167</v>
+        <v>0.1811824291944504</v>
       </c>
       <c r="I84" t="n">
-        <v>0.09823523453254365</v>
+        <v>0.07746239955041412</v>
       </c>
     </row>
     <row r="85">
@@ -3880,10 +3714,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="C85" t="n">
+        <v>29</v>
       </c>
       <c r="D85" t="n">
         <v/>
@@ -3892,7 +3724,7 @@
         <v/>
       </c>
       <c r="F85" t="n">
-        <v>14649951993276.9</v>
+        <v>8540586175314.375</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3900,10 +3732,10 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>0.2212859094142914</v>
+        <v>0.1894466802477837</v>
       </c>
       <c r="I85" t="n">
-        <v>0.1032797624421537</v>
+        <v>0.07758982067393008</v>
       </c>
     </row>
     <row r="86">
@@ -3917,10 +3749,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="C86" t="n">
+        <v>30</v>
       </c>
       <c r="D86" t="n">
         <v/>
@@ -3929,7 +3759,7 @@
         <v/>
       </c>
       <c r="F86" t="n">
-        <v>15083736264262.6</v>
+        <v>8835506630048.125</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3937,10 +3767,10 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>0.2363780364394188</v>
+        <v>0.1947078965604305</v>
       </c>
       <c r="I86" t="n">
-        <v>0.1010852169387407</v>
+        <v>0.07726817402985407</v>
       </c>
     </row>
     <row r="87">
@@ -3954,10 +3784,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="C87" t="n">
+        <v>31</v>
       </c>
       <c r="D87" t="n">
         <v/>
@@ -3966,7 +3794,7 @@
         <v/>
       </c>
       <c r="F87" t="n">
-        <v>11260895825346.33</v>
+        <v>9130049005602.75</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3974,10 +3802,10 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>0.2100706415043937</v>
+        <v>0.1860596518963575</v>
       </c>
       <c r="I87" t="n">
-        <v>0.1055861024071628</v>
+        <v>0.0751374060370233</v>
       </c>
     </row>
     <row r="88">
@@ -3991,10 +3819,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="C88" t="n">
+        <v>32</v>
       </c>
       <c r="D88" t="n">
         <v/>
@@ -4003,7 +3829,7 @@
         <v/>
       </c>
       <c r="F88" t="n">
-        <v>11565086806375.33</v>
+        <v>9425610649249.375</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -4011,10 +3837,10 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>0.2219914197921753</v>
+        <v>0.1834042314440012</v>
       </c>
       <c r="I88" t="n">
-        <v>0.09228428287627098</v>
+        <v>0.07412066476728382</v>
       </c>
     </row>
     <row r="89">
@@ -4028,10 +3854,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="C89" t="n">
+        <v>33</v>
       </c>
       <c r="D89" t="n">
         <v/>
@@ -4040,7 +3864,7 @@
         <v/>
       </c>
       <c r="F89" t="n">
-        <v>11869946863488.33</v>
+        <v>9720738562145.25</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -4048,10 +3872,10 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>0.2176889545387692</v>
+        <v>0.1830331943929195</v>
       </c>
       <c r="I89" t="n">
-        <v>0.09786347507949604</v>
+        <v>0.07274024305692223</v>
       </c>
     </row>
     <row r="90">
@@ -4065,10 +3889,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C90" t="n">
+        <v>34</v>
       </c>
       <c r="D90" t="n">
         <v/>
@@ -4077,7 +3899,7 @@
         <v/>
       </c>
       <c r="F90" t="n">
-        <v>1792281688040.477</v>
+        <v>10014985168236.88</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -4085,10 +3907,10 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>0.2102377187720565</v>
+        <v>0.1986057981848717</v>
       </c>
       <c r="I90" t="n">
-        <v>0.07786842059697734</v>
+        <v>0.07809313348605283</v>
       </c>
     </row>
     <row r="91">
@@ -4102,10 +3924,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="C91" t="n">
+        <v>35</v>
       </c>
       <c r="D91" t="n">
         <v/>
@@ -4114,7 +3934,7 @@
         <v/>
       </c>
       <c r="F91" t="n">
-        <v>12174105762849</v>
+        <v>10309757161148.62</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -4122,10 +3942,10 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>0.2134416417943107</v>
+        <v>0.1833901442587376</v>
       </c>
       <c r="I91" t="n">
-        <v>0.1069798178122482</v>
+        <v>0.07000445209643377</v>
       </c>
     </row>
     <row r="92">
@@ -4139,10 +3959,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="C92" t="n">
+        <v>36</v>
       </c>
       <c r="D92" t="n">
         <v/>
@@ -4151,7 +3969,7 @@
         <v/>
       </c>
       <c r="F92" t="n">
-        <v>12478104119725</v>
+        <v>10604356547791.62</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -4159,10 +3977,10 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>0.2111974391672346</v>
+        <v>0.2031211648136377</v>
       </c>
       <c r="I92" t="n">
-        <v>0.1043608734622792</v>
+        <v>0.07934894647071287</v>
       </c>
     </row>
     <row r="93">
@@ -4176,10 +3994,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="C93" t="n">
+        <v>37</v>
       </c>
       <c r="D93" t="n">
         <v/>
@@ -4188,7 +4004,7 @@
         <v/>
       </c>
       <c r="F93" t="n">
-        <v>12782738037802</v>
+        <v>10898430868917.88</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -4196,10 +4012,10 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>0.225709683365292</v>
+        <v>0.1832808572798967</v>
       </c>
       <c r="I93" t="n">
-        <v>0.1026550015328294</v>
+        <v>0.07320571540825345</v>
       </c>
     </row>
     <row r="94">
@@ -4213,10 +4029,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="C94" t="n">
+        <v>38</v>
       </c>
       <c r="D94" t="n">
         <v/>
@@ -4225,7 +4039,7 @@
         <v/>
       </c>
       <c r="F94" t="n">
-        <v>13085816584195.33</v>
+        <v>11192850655253.25</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -4233,10 +4047,10 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>0.2128185878197352</v>
+        <v>0.2015318423509598</v>
       </c>
       <c r="I94" t="n">
-        <v>0.09872001223562207</v>
+        <v>0.07367139459852201</v>
       </c>
     </row>
     <row r="95">
@@ -4250,10 +4064,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="C95" t="n">
+        <v>39</v>
       </c>
       <c r="D95" t="n">
         <v/>
@@ -4262,7 +4074,7 @@
         <v/>
       </c>
       <c r="F95" t="n">
-        <v>13390352748868.55</v>
+        <v>11487881847928.25</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -4270,10 +4082,10 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>0.219504016968939</v>
+        <v>0.1930310986936092</v>
       </c>
       <c r="I95" t="n">
-        <v>0.1018652930164572</v>
+        <v>0.06849543101099262</v>
       </c>
     </row>
     <row r="96">
@@ -4287,10 +4099,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="C96" t="n">
+        <v>40</v>
       </c>
       <c r="D96" t="n">
         <v/>
@@ -4299,7 +4109,7 @@
         <v/>
       </c>
       <c r="F96" t="n">
-        <v>13695505748551.45</v>
+        <v>11782250415032.88</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -4307,10 +4117,10 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>0.2109212279319763</v>
+        <v>0.1859051492065191</v>
       </c>
       <c r="I96" t="n">
-        <v>0.1081449753835664</v>
+        <v>0.07266640491454728</v>
       </c>
     </row>
     <row r="97">
@@ -4324,10 +4134,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
+      <c r="C97" t="n">
+        <v>41</v>
       </c>
       <c r="D97" t="n">
         <v/>
@@ -4336,7 +4144,7 @@
         <v/>
       </c>
       <c r="F97" t="n">
-        <v>14000529518542</v>
+        <v>12076338097233.5</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -4344,10 +4152,10 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>0.2252375930547714</v>
+        <v>0.1851323656737804</v>
       </c>
       <c r="I97" t="n">
-        <v>0.1023223743377557</v>
+        <v>0.07388562128693886</v>
       </c>
     </row>
     <row r="98">
@@ -4361,10 +4169,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="C98" t="n">
+        <v>42</v>
       </c>
       <c r="D98" t="n">
         <v/>
@@ -4373,7 +4179,7 @@
         <v/>
       </c>
       <c r="F98" t="n">
-        <v>14397679048431.25</v>
+        <v>12371093313572.25</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -4381,10 +4187,10 @@
         </is>
       </c>
       <c r="H98" t="n">
-        <v>0.2187952976673841</v>
+        <v>0.2013100646436214</v>
       </c>
       <c r="I98" t="n">
-        <v>0.1126390912355293</v>
+        <v>0.07694136391408077</v>
       </c>
     </row>
     <row r="99">
@@ -4398,10 +4204,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="C99" t="n">
+        <v>43</v>
       </c>
       <c r="D99" t="n">
         <v/>
@@ -4410,7 +4214,7 @@
         <v/>
       </c>
       <c r="F99" t="n">
-        <v>14704699205883.62</v>
+        <v>12664229246068.62</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -4418,10 +4222,10 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>0.217534676194191</v>
+        <v>0.1888273973017931</v>
       </c>
       <c r="I99" t="n">
-        <v>0.09397970016080291</v>
+        <v>0.07223331889360922</v>
       </c>
     </row>
     <row r="100">
@@ -4435,10 +4239,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="C100" t="n">
+        <v>44</v>
       </c>
       <c r="D100" t="n">
         <v/>
@@ -4447,7 +4249,7 @@
         <v/>
       </c>
       <c r="F100" t="n">
-        <v>15010773351995.88</v>
+        <v>12959012243525.38</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -4455,10 +4257,10 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>0.2212605029344559</v>
+        <v>0.1938723269850016</v>
       </c>
       <c r="I100" t="n">
-        <v>0.1141187503044984</v>
+        <v>0.07142377466069931</v>
       </c>
     </row>
     <row r="101">
@@ -4472,10 +4274,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C101" t="n">
+        <v>45</v>
       </c>
       <c r="D101" t="n">
         <v/>
@@ -4484,7 +4284,7 @@
         <v/>
       </c>
       <c r="F101" t="n">
-        <v>2248899399984.635</v>
+        <v>13254366729402.88</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -4492,10 +4292,10 @@
         </is>
       </c>
       <c r="H101" t="n">
-        <v>0.216755330211976</v>
+        <v>0.1829858161509037</v>
       </c>
       <c r="I101" t="n">
-        <v>0.08362528499461744</v>
+        <v>0.07307022546493488</v>
       </c>
     </row>
     <row r="102">
@@ -4509,10 +4309,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="C102" t="n">
+        <v>46</v>
       </c>
       <c r="D102" t="n">
         <v/>
@@ -4521,7 +4319,7 @@
         <v/>
       </c>
       <c r="F102" t="n">
-        <v>15317779067481.5</v>
+        <v>13549649047011.5</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4529,10 +4327,10 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>0.226020434871316</v>
+        <v>0.1999342571943998</v>
       </c>
       <c r="I102" t="n">
-        <v>0.09763206193254741</v>
+        <v>0.07334878742128237</v>
       </c>
     </row>
     <row r="103">
@@ -4546,10 +4344,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="C103" t="n">
+        <v>47</v>
       </c>
       <c r="D103" t="n">
         <v/>
@@ -4558,7 +4354,7 @@
         <v/>
       </c>
       <c r="F103" t="n">
-        <v>2398735748890.25</v>
+        <v>13884469149822.86</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4566,10 +4362,10 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>0.183305108298858</v>
+        <v>0.187964283994266</v>
       </c>
       <c r="I103" t="n">
-        <v>0.06191742958850368</v>
+        <v>0.07700873921217133</v>
       </c>
     </row>
     <row r="104">
@@ -4583,10 +4379,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C104" t="n">
+        <v>48</v>
       </c>
       <c r="D104" t="n">
         <v/>
@@ -4595,7 +4389,7 @@
         <v/>
       </c>
       <c r="F104" t="n">
-        <v>2798004037576.25</v>
+        <v>14180589981977.43</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4603,10 +4397,10 @@
         </is>
       </c>
       <c r="H104" t="n">
-        <v>0.1882850701610247</v>
+        <v>0.1948428196566445</v>
       </c>
       <c r="I104" t="n">
-        <v>0.07056594385056314</v>
+        <v>0.07415046473381895</v>
       </c>
     </row>
     <row r="105">
@@ -4620,10 +4414,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="C105" t="n">
+        <v>49</v>
       </c>
       <c r="D105" t="n">
         <v/>
@@ -4632,7 +4424,7 @@
         <v/>
       </c>
       <c r="F105" t="n">
-        <v>3197894582411.417</v>
+        <v>14475943991165</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4640,10 +4432,10 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>0.1870441511273384</v>
+        <v>0.1905131680624826</v>
       </c>
       <c r="I105" t="n">
-        <v>0.07681432432930396</v>
+        <v>0.07981155148283595</v>
       </c>
     </row>
     <row r="106">
@@ -4657,10 +4449,8 @@
           <t>coco</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C106" t="n">
+        <v>50</v>
       </c>
       <c r="D106" t="n">
         <v/>
@@ -4669,7 +4459,7 @@
         <v/>
       </c>
       <c r="F106" t="n">
-        <v>3597584389032.583</v>
+        <v>14771778885317.57</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4677,10 +4467,10 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>0.1821188113341729</v>
+        <v>0.202729657292366</v>
       </c>
       <c r="I106" t="n">
-        <v>0.08444873575037527</v>
+        <v>0.07783139757129603</v>
       </c>
       <c r="V106" t="inlineStr">
         <is>

</xml_diff>